<commit_message>
Alteracao da Base de Dados de Treinamento dos Medicos
</commit_message>
<xml_diff>
--- a/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
+++ b/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E66498F-A268-4693-96C8-35FA8FA3F2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916EBD15-3686-4E68-AFE4-270CE1660883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F52E2CE3-F2BB-45A9-B9E9-D8B91065BEDA}"/>
   </bookViews>
@@ -1254,7 +1254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1452,6 +1452,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1487,21 +1490,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1821,11 +1809,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z669"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y131" sqref="Y131"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2614,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>58</v>
       </c>
@@ -3228,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>76</v>
       </c>
@@ -3342,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>78</v>
       </c>
@@ -3582,7 +3571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>84</v>
       </c>
@@ -3637,7 +3626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>85</v>
       </c>
@@ -3755,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>89</v>
       </c>
@@ -3810,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>90</v>
       </c>
@@ -4117,7 +4106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>96</v>
       </c>
@@ -4172,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>97</v>
       </c>
@@ -4353,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>101</v>
       </c>
@@ -4912,7 +4901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>118</v>
       </c>
@@ -5156,7 +5145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="66" t="s">
         <v>126</v>
       </c>
@@ -5333,7 +5322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="66" t="s">
         <v>130</v>
       </c>
@@ -5384,7 +5373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="66" t="s">
         <v>132</v>
       </c>
@@ -5435,7 +5424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="66" t="s">
         <v>133</v>
       </c>
@@ -5612,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="66" t="s">
         <v>139</v>
       </c>
@@ -5667,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="66" t="s">
         <v>141</v>
       </c>
@@ -5722,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="66" t="s">
         <v>142</v>
       </c>
@@ -5775,7 +5764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="66" t="s">
         <v>143</v>
       </c>
@@ -5828,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="66" t="s">
         <v>144</v>
       </c>
@@ -5944,7 +5933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="66" t="s">
         <v>146</v>
       </c>
@@ -5997,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="66" t="s">
         <v>147</v>
       </c>
@@ -6052,7 +6041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="66" t="s">
         <v>148</v>
       </c>
@@ -6105,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="66" t="s">
         <v>149</v>
       </c>
@@ -6160,7 +6149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="66" t="s">
         <v>150</v>
       </c>
@@ -6215,7 +6204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="66" t="s">
         <v>151</v>
       </c>
@@ -6270,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="66" t="s">
         <v>152</v>
       </c>
@@ -6388,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="66" t="s">
         <v>154</v>
       </c>
@@ -6443,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="66" t="s">
         <v>155</v>
       </c>
@@ -6498,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="66" t="s">
         <v>156</v>
       </c>
@@ -6553,70 +6542,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="88" t="s">
+    <row r="80" spans="1:25" s="102" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="89" t="s">
+      <c r="B80" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="C80" s="90" t="s">
+      <c r="C80" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="D80" s="91" t="s">
+      <c r="D80" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="E80" s="90"/>
-      <c r="F80" s="90"/>
-      <c r="G80" s="90" t="s">
+      <c r="E80" s="91"/>
+      <c r="F80" s="91"/>
+      <c r="G80" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="H80" s="92">
+      <c r="H80" s="93">
         <v>45175</v>
       </c>
-      <c r="I80" s="93" t="s">
+      <c r="I80" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="J80" s="92" t="s">
+      <c r="J80" s="93" t="s">
         <v>158</v>
       </c>
-      <c r="K80" s="92" t="s">
+      <c r="K80" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="L80" s="94"/>
-      <c r="M80" s="94"/>
-      <c r="N80" s="94"/>
-      <c r="O80" s="95" t="s">
+      <c r="L80" s="95"/>
+      <c r="M80" s="95"/>
+      <c r="N80" s="95"/>
+      <c r="O80" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="P80" s="96">
+      <c r="P80" s="97">
         <v>45261</v>
       </c>
-      <c r="Q80" s="89" t="s">
+      <c r="Q80" s="90" t="s">
         <v>159</v>
       </c>
-      <c r="R80" s="97">
+      <c r="R80" s="98">
         <v>45261</v>
       </c>
-      <c r="S80" s="98" t="s">
+      <c r="S80" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="T80" s="98" t="s">
+      <c r="T80" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="U80" s="98"/>
-      <c r="V80" s="98"/>
-      <c r="W80" s="99" t="s">
+      <c r="U80" s="99"/>
+      <c r="V80" s="99"/>
+      <c r="W80" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="X80" s="100" t="s">
+      <c r="X80" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="Y80" s="100">
+      <c r="Y80" s="101">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="71" t="s">
         <v>160</v>
       </c>
@@ -7112,7 +7101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="15" t="s">
         <v>172</v>
       </c>
@@ -7230,7 +7219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
         <v>175</v>
       </c>
@@ -7285,7 +7274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="15" t="s">
         <v>176</v>
       </c>
@@ -7340,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>177</v>
       </c>
@@ -7395,7 +7384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>132</v>
       </c>
@@ -7446,7 +7435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
         <v>180</v>
       </c>
@@ -7501,7 +7490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>181</v>
       </c>
@@ -7556,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
         <v>182</v>
       </c>
@@ -7737,7 +7726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
         <v>185</v>
       </c>
@@ -7790,7 +7779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="15" t="s">
         <v>187</v>
       </c>
@@ -7908,7 +7897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="67" t="s">
         <v>224</v>
       </c>
@@ -7963,7 +7952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
         <v>225</v>
       </c>
@@ -8018,7 +8007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="67" t="s">
         <v>189</v>
       </c>
@@ -8073,7 +8062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="67" t="s">
         <v>190</v>
       </c>
@@ -8128,7 +8117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="15" t="s">
         <v>192</v>
       </c>
@@ -8183,7 +8172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="15" t="s">
         <v>193</v>
       </c>
@@ -8238,7 +8227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="15" t="s">
         <v>194</v>
       </c>
@@ -8293,7 +8282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="15" t="s">
         <v>195</v>
       </c>
@@ -8348,7 +8337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
         <v>196</v>
       </c>
@@ -8403,129 +8392,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="89" t="s">
+    <row r="112" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="B112" s="89" t="s">
+      <c r="B112" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C112" s="90" t="s">
+      <c r="C112" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D112" s="91" t="s">
+      <c r="D112" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E112" s="90"/>
-      <c r="F112" s="90"/>
-      <c r="G112" s="90" t="s">
+      <c r="E112" s="20"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H112" s="92">
+      <c r="H112" s="32">
         <v>45293</v>
       </c>
-      <c r="I112" s="93" t="s">
+      <c r="I112" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="J112" s="102" t="s">
+      <c r="J112" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="K112" s="92" t="s">
+      <c r="K112" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L112" s="94"/>
-      <c r="M112" s="94"/>
-      <c r="N112" s="94"/>
-      <c r="O112" s="94" t="s">
+      <c r="L112" s="60"/>
+      <c r="M112" s="60"/>
+      <c r="N112" s="60"/>
+      <c r="O112" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="P112" s="92">
+      <c r="P112" s="32">
         <v>45359</v>
       </c>
-      <c r="Q112" s="89"/>
-      <c r="R112" s="103">
+      <c r="Q112" s="15"/>
+      <c r="R112" s="48">
         <v>45359</v>
       </c>
-      <c r="S112" s="104" t="s">
+      <c r="S112" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="T112" s="98" t="s">
+      <c r="T112" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="U112" s="105"/>
-      <c r="V112" s="105"/>
-      <c r="W112" s="99" t="s">
+      <c r="U112" s="73"/>
+      <c r="V112" s="73"/>
+      <c r="W112" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X112" s="100" t="s">
+      <c r="X112" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y112" s="100">
+      <c r="Y112" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="89" t="s">
+    <row r="113" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="B113" s="89" t="s">
+      <c r="B113" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C113" s="90" t="s">
+      <c r="C113" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D113" s="106" t="s">
+      <c r="D113" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E113" s="90"/>
-      <c r="F113" s="90"/>
-      <c r="G113" s="90" t="s">
+      <c r="E113" s="20"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H113" s="92">
+      <c r="H113" s="32">
         <v>45299</v>
       </c>
-      <c r="I113" s="107" t="s">
+      <c r="I113" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="J113" s="92" t="s">
+      <c r="J113" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="K113" s="95" t="s">
+      <c r="K113" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="L113" s="94"/>
-      <c r="M113" s="94"/>
-      <c r="N113" s="94"/>
-      <c r="O113" s="95" t="s">
+      <c r="L113" s="60"/>
+      <c r="M113" s="60"/>
+      <c r="N113" s="60"/>
+      <c r="O113" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="P113" s="92">
+      <c r="P113" s="32">
         <v>45331</v>
       </c>
-      <c r="Q113" s="89"/>
-      <c r="R113" s="103">
+      <c r="Q113" s="15"/>
+      <c r="R113" s="48">
         <v>45331</v>
       </c>
-      <c r="S113" s="98" t="s">
+      <c r="S113" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="T113" s="95" t="s">
+      <c r="T113" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="U113" s="105"/>
-      <c r="V113" s="105"/>
-      <c r="W113" s="99" t="s">
+      <c r="U113" s="73"/>
+      <c r="V113" s="73"/>
+      <c r="W113" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X113" s="100" t="s">
+      <c r="X113" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y113" s="100">
+      <c r="Y113" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="15" t="s">
         <v>199</v>
       </c>
@@ -8584,7 +8573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
         <v>200</v>
       </c>
@@ -8637,7 +8626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:25" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
         <v>201</v>
       </c>
@@ -8692,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
         <v>226</v>
       </c>
@@ -8747,7 +8736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
         <v>202</v>
       </c>
@@ -8802,7 +8791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
         <v>203</v>
       </c>
@@ -8857,7 +8846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="15" t="s">
         <v>204</v>
       </c>
@@ -8912,68 +8901,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="89" t="s">
+    <row r="121" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="B121" s="89" t="s">
+      <c r="B121" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C121" s="90" t="s">
+      <c r="C121" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D121" s="91" t="s">
+      <c r="D121" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E121" s="90"/>
-      <c r="F121" s="90"/>
-      <c r="G121" s="90" t="s">
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H121" s="92">
+      <c r="H121" s="32">
         <v>45317</v>
       </c>
-      <c r="I121" s="107" t="s">
+      <c r="I121" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="J121" s="92" t="s">
+      <c r="J121" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="K121" s="92" t="s">
+      <c r="K121" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L121" s="94"/>
-      <c r="M121" s="94"/>
-      <c r="N121" s="94"/>
-      <c r="O121" s="94" t="s">
+      <c r="L121" s="60"/>
+      <c r="M121" s="60"/>
+      <c r="N121" s="60"/>
+      <c r="O121" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="P121" s="92">
+      <c r="P121" s="32">
         <v>45337</v>
       </c>
-      <c r="Q121" s="89"/>
-      <c r="R121" s="103">
+      <c r="Q121" s="15"/>
+      <c r="R121" s="48">
         <v>45337</v>
       </c>
-      <c r="S121" s="98" t="s">
+      <c r="S121" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="T121" s="95" t="s">
+      <c r="T121" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="U121" s="105"/>
-      <c r="V121" s="105"/>
-      <c r="W121" s="99" t="s">
+      <c r="U121" s="73"/>
+      <c r="V121" s="73"/>
+      <c r="W121" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X121" s="100" t="s">
+      <c r="X121" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y121" s="100">
+      <c r="Y121" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
         <v>206</v>
       </c>
@@ -9028,68 +9017,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="89" t="s">
+    <row r="123" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="B123" s="89" t="s">
+      <c r="B123" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C123" s="90" t="s">
+      <c r="C123" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D123" s="106" t="s">
+      <c r="D123" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E123" s="90"/>
-      <c r="F123" s="90"/>
-      <c r="G123" s="90" t="s">
+      <c r="E123" s="20"/>
+      <c r="F123" s="20"/>
+      <c r="G123" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H123" s="92">
+      <c r="H123" s="32">
         <v>45320</v>
       </c>
-      <c r="I123" s="93" t="s">
+      <c r="I123" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="J123" s="92" t="s">
+      <c r="J123" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="K123" s="92" t="s">
+      <c r="K123" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L123" s="94"/>
-      <c r="M123" s="94"/>
-      <c r="N123" s="94"/>
-      <c r="O123" s="95" t="s">
+      <c r="L123" s="60"/>
+      <c r="M123" s="60"/>
+      <c r="N123" s="60"/>
+      <c r="O123" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="P123" s="92">
+      <c r="P123" s="32">
         <v>45352</v>
       </c>
-      <c r="Q123" s="89"/>
-      <c r="R123" s="103">
+      <c r="Q123" s="15"/>
+      <c r="R123" s="48">
         <v>45352</v>
       </c>
-      <c r="S123" s="104" t="s">
+      <c r="S123" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="T123" s="98" t="s">
+      <c r="T123" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="U123" s="105"/>
-      <c r="V123" s="105"/>
-      <c r="W123" s="99" t="s">
+      <c r="U123" s="73"/>
+      <c r="V123" s="73"/>
+      <c r="W123" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X123" s="100" t="s">
+      <c r="X123" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y123" s="100">
+      <c r="Y123" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="67" t="s">
         <v>207</v>
       </c>
@@ -9144,7 +9133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="15" t="s">
         <v>208</v>
       </c>
@@ -9199,7 +9188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="15" t="s">
         <v>209</v>
       </c>
@@ -9254,68 +9243,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="89" t="s">
+    <row r="127" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="B127" s="89" t="s">
+      <c r="B127" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C127" s="90" t="s">
+      <c r="C127" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D127" s="106" t="s">
+      <c r="D127" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E127" s="90"/>
-      <c r="F127" s="90"/>
-      <c r="G127" s="90" t="s">
+      <c r="E127" s="20"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H127" s="92">
+      <c r="H127" s="32">
         <v>45325</v>
       </c>
-      <c r="I127" s="93" t="s">
+      <c r="I127" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="J127" s="92" t="s">
+      <c r="J127" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="K127" s="92" t="s">
+      <c r="K127" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L127" s="94"/>
-      <c r="M127" s="94"/>
-      <c r="N127" s="94"/>
-      <c r="O127" s="108" t="s">
+      <c r="L127" s="60"/>
+      <c r="M127" s="60"/>
+      <c r="N127" s="60"/>
+      <c r="O127" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="P127" s="92">
+      <c r="P127" s="32">
         <v>45342</v>
       </c>
-      <c r="Q127" s="89"/>
-      <c r="R127" s="103">
+      <c r="Q127" s="15"/>
+      <c r="R127" s="48">
         <v>45342</v>
       </c>
-      <c r="S127" s="98" t="s">
+      <c r="S127" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="T127" s="95" t="s">
+      <c r="T127" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="U127" s="105"/>
-      <c r="V127" s="105"/>
-      <c r="W127" s="99" t="s">
+      <c r="U127" s="73"/>
+      <c r="V127" s="73"/>
+      <c r="W127" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X127" s="100" t="s">
+      <c r="X127" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y127" s="100">
+      <c r="Y127" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:25" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="79" t="s">
         <v>211</v>
       </c>
@@ -9437,129 +9426,129 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="89" t="s">
+    <row r="130" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B130" s="89" t="s">
+      <c r="B130" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C130" s="90" t="s">
+      <c r="C130" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D130" s="106" t="s">
+      <c r="D130" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E130" s="90"/>
-      <c r="F130" s="90"/>
-      <c r="G130" s="90" t="s">
+      <c r="E130" s="20"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H130" s="92">
+      <c r="H130" s="32">
         <v>45333</v>
       </c>
-      <c r="I130" s="93" t="s">
+      <c r="I130" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="J130" s="92" t="s">
+      <c r="J130" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="K130" s="92" t="s">
+      <c r="K130" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L130" s="94"/>
-      <c r="M130" s="94"/>
-      <c r="N130" s="94"/>
-      <c r="O130" s="95" t="s">
+      <c r="L130" s="60"/>
+      <c r="M130" s="60"/>
+      <c r="N130" s="60"/>
+      <c r="O130" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="P130" s="92">
+      <c r="P130" s="32">
         <v>45358</v>
       </c>
-      <c r="Q130" s="89"/>
-      <c r="R130" s="103">
+      <c r="Q130" s="15"/>
+      <c r="R130" s="48">
         <v>45358</v>
       </c>
-      <c r="S130" s="98" t="s">
+      <c r="S130" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="T130" s="95" t="s">
+      <c r="T130" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="U130" s="105"/>
-      <c r="V130" s="105"/>
-      <c r="W130" s="99" t="s">
+      <c r="U130" s="73"/>
+      <c r="V130" s="73"/>
+      <c r="W130" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X130" s="100" t="s">
+      <c r="X130" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y130" s="100">
+      <c r="Y130" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:25" s="101" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="89" t="s">
+    <row r="131" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="B131" s="89" t="s">
+      <c r="B131" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C131" s="90" t="s">
+      <c r="C131" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D131" s="106" t="s">
+      <c r="D131" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E131" s="90"/>
-      <c r="F131" s="90"/>
-      <c r="G131" s="90" t="s">
+      <c r="E131" s="20"/>
+      <c r="F131" s="20"/>
+      <c r="G131" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H131" s="92">
+      <c r="H131" s="32">
         <v>45325</v>
       </c>
-      <c r="I131" s="93" t="s">
+      <c r="I131" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="J131" s="92" t="s">
+      <c r="J131" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="K131" s="92" t="s">
+      <c r="K131" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L131" s="94"/>
-      <c r="M131" s="94"/>
-      <c r="N131" s="94"/>
-      <c r="O131" s="95" t="s">
+      <c r="L131" s="60"/>
+      <c r="M131" s="60"/>
+      <c r="N131" s="60"/>
+      <c r="O131" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="P131" s="92">
+      <c r="P131" s="32">
         <v>45352</v>
       </c>
-      <c r="Q131" s="89"/>
-      <c r="R131" s="103">
+      <c r="Q131" s="15"/>
+      <c r="R131" s="48">
         <v>45352</v>
       </c>
-      <c r="S131" s="98" t="s">
+      <c r="S131" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="T131" s="95" t="s">
+      <c r="T131" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="U131" s="105"/>
-      <c r="V131" s="105"/>
-      <c r="W131" s="99" t="s">
+      <c r="U131" s="73"/>
+      <c r="V131" s="73"/>
+      <c r="W131" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X131" s="100" t="s">
+      <c r="X131" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y131" s="100">
+      <c r="Y131" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="15" t="s">
         <v>229</v>
       </c>
@@ -9614,7 +9603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="15" t="s">
         <v>230</v>
       </c>
@@ -9667,7 +9656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="15" t="s">
         <v>231</v>
       </c>
@@ -9720,7 +9709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="15" t="s">
         <v>232</v>
       </c>
@@ -9773,7 +9762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="15" t="s">
         <v>233</v>
       </c>
@@ -24643,7 +24632,13 @@
       <c r="Z669" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z136" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}"/>
+  <autoFilter ref="A1:Z136" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
+    <filterColumn colId="18">
+      <filters>
+        <filter val="REALIZADO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -34188,10 +34183,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="87"/>
+      <c r="B1" s="88"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -34229,15 +34224,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7271154-468d-4943-ad07-15f269a1f4f5" xsi:nil="true"/>
@@ -34246,6 +34232,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34498,20 +34493,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828E50A0-1F61-4B82-AF91-2402CEF44BFC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f7271154-468d-4943-ad07-15f269a1f4f5"/>
     <ds:schemaRef ds:uri="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Atualizacao da Base de Dados Treinamento dos Medicos
</commit_message>
<xml_diff>
--- a/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
+++ b/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916EBD15-3686-4E68-AFE4-270CE1660883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82724EB3-CDF0-4B84-B674-586872B701D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F52E2CE3-F2BB-45A9-B9E9-D8B91065BEDA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F52E2CE3-F2BB-45A9-B9E9-D8B91065BEDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados_Onboarding" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="SLAs" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados_Onboarding!$A$1:$Z$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados_Onboarding!$A$1:$Z$138</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="273">
   <si>
     <t>Nome do Médico</t>
   </si>
@@ -688,10 +688,6 @@
     <t>Juliana Mathias Netto Khouri</t>
   </si>
   <si>
-    <t>-&gt;SIM.
--&gt;Email do médico estava sem o domínio " @medicos.oncoclinicas.com"</t>
-  </si>
-  <si>
     <t>Karina Hatsumi Miyake</t>
   </si>
   <si>
@@ -999,6 +995,48 @@
   <si>
     <t>-&gt;Não foi encontrada uma caixa postal para o e-mail do médico</t>
   </si>
+  <si>
+    <t>Fabiola Assad Antunes</t>
+  </si>
+  <si>
+    <t>01/01/0000</t>
+  </si>
+  <si>
+    <t>-&gt;E-mail do Médico com domínio "@oncoclinicas.com"
+-&gt;Médico Satélite no grupo de médico Híbrido
+-&gt;Cadastro Completo de Pessoa no Tasy está sem "CPF" e sem "Data de Nascimento" - 
+(Não foi possível realizar a correção do cadastro pois o consultor ainda não enviou os dados faltantes do médico</t>
+  </si>
+  <si>
+    <t>❇ CRITÍCA
+➡️ Médico informou que ele vai perder muito tempo da consulta realizando essa parte burocrática
+➡️ Médico informou que ele não vai realizar o procedimento</t>
+  </si>
+  <si>
+    <t>-&gt;Médico preferiu não informar no momento</t>
+  </si>
+  <si>
+    <t>❇ CRITÍCA
+➡️ Médico informou que essa parte é burocrática, mas não informou objeção</t>
+  </si>
+  <si>
+    <t>-&gt;Medico solicitou que aguardassemos o mesmo ter paciente para o encaminhamento.</t>
+  </si>
+  <si>
+    <t>❇ SUGESTÃO
+➡️ Médico informou que seria bom se o paciente levasse os documentos pessoais para o concierge
+❇ CRITÍCA
+➡️ Médico informou que pode perder muito tempo da consulta realizando essa parte burocrática</t>
+  </si>
+  <si>
+    <t>➡️ Médico preferiu não informar</t>
+  </si>
+  <si>
+    <t>Janaina Michelle Lima Melo</t>
+  </si>
+  <si>
+    <t>Carla Libralli Tostes dos Santos</t>
+  </si>
 </sst>
 </file>
 
@@ -1254,7 +1292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1440,56 +1478,95 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1809,12 +1886,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z669"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80:XFD80"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1913,13 +1989,13 @@
         <v>21</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X1" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y1" s="27" t="s">
         <v>221</v>
-      </c>
-      <c r="Y1" s="27" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -1944,7 +2020,7 @@
         <v>45247</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J2" s="34" t="s">
         <v>26</v>
@@ -2007,7 +2083,7 @@
         <v>45246</v>
       </c>
       <c r="I3" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J3" s="43" t="s">
         <v>36</v>
@@ -2068,7 +2144,7 @@
         <v>45256</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J4" s="34" t="s">
         <v>39</v>
@@ -2131,7 +2207,7 @@
         <v>45213</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J5" s="34" t="s">
         <v>44</v>
@@ -2192,7 +2268,7 @@
         <v>45257</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J6" s="43" t="s">
         <v>46</v>
@@ -2253,7 +2329,7 @@
         <v>45240</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J7" s="43" t="s">
         <v>46</v>
@@ -2316,7 +2392,7 @@
         <v>45246</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J8" s="43" t="s">
         <v>46</v>
@@ -2377,7 +2453,7 @@
         <v>45233</v>
       </c>
       <c r="I9" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J9" s="32" t="s">
         <v>52</v>
@@ -2440,7 +2516,7 @@
         <v>45254</v>
       </c>
       <c r="I10" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J10" s="32" t="s">
         <v>52</v>
@@ -2501,7 +2577,7 @@
         <v>45233</v>
       </c>
       <c r="I11" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J11" s="32" t="s">
         <v>52</v>
@@ -2562,7 +2638,7 @@
         <v>45224</v>
       </c>
       <c r="I12" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J12" s="32" t="s">
         <v>52</v>
@@ -2603,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>58</v>
       </c>
@@ -2625,7 +2701,7 @@
         <v>45261</v>
       </c>
       <c r="I13" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J13" s="32" t="s">
         <v>52</v>
@@ -2640,14 +2716,14 @@
         <v>59</v>
       </c>
       <c r="P13" s="32">
-        <v>45373</v>
+        <v>45387</v>
       </c>
       <c r="Q13" s="15" t="s">
         <v>60</v>
       </c>
       <c r="R13" s="52"/>
-      <c r="S13" s="49" t="s">
-        <v>213</v>
+      <c r="S13" s="101" t="s">
+        <v>212</v>
       </c>
       <c r="T13" s="49"/>
       <c r="U13" s="53"/>
@@ -2682,7 +2758,7 @@
         <v>45233</v>
       </c>
       <c r="I14" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J14" s="32" t="s">
         <v>52</v>
@@ -2745,7 +2821,7 @@
         <v>45226</v>
       </c>
       <c r="I15" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J15" s="32" t="s">
         <v>52</v>
@@ -2806,7 +2882,7 @@
         <v>45252</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J16" s="32" t="s">
         <v>66</v>
@@ -2869,7 +2945,7 @@
         <v>45252</v>
       </c>
       <c r="I17" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J17" s="32" t="s">
         <v>69</v>
@@ -2930,7 +3006,7 @@
         <v>45260</v>
       </c>
       <c r="I18" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J18" s="34" t="s">
         <v>39</v>
@@ -2993,7 +3069,7 @@
         <v>45258</v>
       </c>
       <c r="I19" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J19" s="32" t="s">
         <v>52</v>
@@ -3054,7 +3130,7 @@
         <v>45260</v>
       </c>
       <c r="I20" s="56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J20" s="32" t="s">
         <v>66</v>
@@ -3115,7 +3191,7 @@
         <v>45104</v>
       </c>
       <c r="I21" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J21" s="43" t="s">
         <v>46</v>
@@ -3176,7 +3252,7 @@
         <v>45224</v>
       </c>
       <c r="I22" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J22" s="32" t="s">
         <v>52</v>
@@ -3217,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>76</v>
       </c>
@@ -3239,7 +3315,7 @@
         <v>45260</v>
       </c>
       <c r="I23" s="56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J23" s="32" t="s">
         <v>66</v>
@@ -3290,7 +3366,7 @@
         <v>45218</v>
       </c>
       <c r="I24" s="56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J24" s="32" t="s">
         <v>66</v>
@@ -3331,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>78</v>
       </c>
@@ -3353,7 +3429,7 @@
         <v>45211</v>
       </c>
       <c r="I25" s="56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J25" s="32" t="s">
         <v>66</v>
@@ -3404,7 +3480,7 @@
         <v>45271</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J26" s="32" t="s">
         <v>39</v>
@@ -3467,7 +3543,7 @@
         <v>45260</v>
       </c>
       <c r="I27" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J27" s="32" t="s">
         <v>39</v>
@@ -3530,7 +3606,7 @@
         <v>45246</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J28" s="32" t="s">
         <v>39</v>
@@ -3571,7 +3647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>84</v>
       </c>
@@ -3593,7 +3669,7 @@
         <v>45248</v>
       </c>
       <c r="I29" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J29" s="32" t="s">
         <v>39</v>
@@ -3608,7 +3684,7 @@
         <v>71</v>
       </c>
       <c r="P29" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q29" s="15"/>
       <c r="R29" s="52"/>
@@ -3626,58 +3702,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
+    <row r="30" spans="1:25" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20" t="s">
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="32">
+      <c r="H30" s="88">
         <v>45247</v>
       </c>
-      <c r="I30" s="33" t="s">
-        <v>238</v>
-      </c>
-      <c r="J30" s="32" t="s">
+      <c r="I30" s="122" t="s">
+        <v>237</v>
+      </c>
+      <c r="J30" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="K30" s="32" t="s">
+      <c r="K30" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36"/>
-      <c r="O30" s="60" t="s">
+      <c r="L30" s="89"/>
+      <c r="M30" s="89"/>
+      <c r="N30" s="89"/>
+      <c r="O30" s="123" t="s">
         <v>86</v>
       </c>
-      <c r="P30" s="32" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="52"/>
-      <c r="S30" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="T30" s="49"/>
-      <c r="U30" s="49"/>
-      <c r="V30" s="49"/>
-      <c r="W30" s="40" t="s">
+      <c r="P30" s="88">
+        <v>45386</v>
+      </c>
+      <c r="Q30" s="86"/>
+      <c r="R30" s="117"/>
+      <c r="S30" s="118" t="s">
+        <v>212</v>
+      </c>
+      <c r="T30" s="118"/>
+      <c r="U30" s="118"/>
+      <c r="V30" s="118"/>
+      <c r="W30" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="X30" s="55"/>
-      <c r="Y30" s="28">
+      <c r="X30" s="120"/>
+      <c r="Y30" s="90">
         <v>0</v>
       </c>
     </row>
@@ -3703,7 +3779,7 @@
         <v>45233</v>
       </c>
       <c r="I31" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J31" s="32" t="s">
         <v>39</v>
@@ -3744,7 +3820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>89</v>
       </c>
@@ -3766,7 +3842,7 @@
         <v>45261</v>
       </c>
       <c r="I32" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J32" s="32" t="s">
         <v>39</v>
@@ -3781,7 +3857,7 @@
         <v>71</v>
       </c>
       <c r="P32" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q32" s="15"/>
       <c r="R32" s="52"/>
@@ -3799,7 +3875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>90</v>
       </c>
@@ -3821,7 +3897,7 @@
         <v>45236</v>
       </c>
       <c r="I33" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J33" s="32" t="s">
         <v>39</v>
@@ -3836,7 +3912,7 @@
         <v>83</v>
       </c>
       <c r="P33" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q33" s="15"/>
       <c r="R33" s="52"/>
@@ -3876,7 +3952,7 @@
         <v>45247</v>
       </c>
       <c r="I34" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J34" s="32" t="s">
         <v>39</v>
@@ -3939,7 +4015,7 @@
         <v>45225</v>
       </c>
       <c r="I35" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J35" s="32" t="s">
         <v>39</v>
@@ -4002,7 +4078,7 @@
         <v>45260</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J36" s="32" t="s">
         <v>39</v>
@@ -4065,7 +4141,7 @@
         <v>45226</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J37" s="32" t="s">
         <v>39</v>
@@ -4106,7 +4182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>96</v>
       </c>
@@ -4128,7 +4204,7 @@
         <v>45247</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J38" s="32" t="s">
         <v>39</v>
@@ -4143,7 +4219,7 @@
         <v>27</v>
       </c>
       <c r="P38" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q38" s="15"/>
       <c r="R38" s="52"/>
@@ -4161,7 +4237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>97</v>
       </c>
@@ -4183,7 +4259,7 @@
         <v>45233</v>
       </c>
       <c r="I39" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J39" s="32" t="s">
         <v>39</v>
@@ -4238,7 +4314,7 @@
         <v>45247</v>
       </c>
       <c r="I40" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J40" s="32" t="s">
         <v>39</v>
@@ -4301,7 +4377,7 @@
         <v>45260</v>
       </c>
       <c r="I41" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J41" s="32" t="s">
         <v>39</v>
@@ -4342,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>101</v>
       </c>
@@ -4364,7 +4440,7 @@
         <v>45233</v>
       </c>
       <c r="I42" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J42" s="32" t="s">
         <v>39</v>
@@ -4379,7 +4455,7 @@
         <v>80</v>
       </c>
       <c r="P42" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="52"/>
@@ -4419,7 +4495,7 @@
         <v>45268</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J43" s="32" t="s">
         <v>39</v>
@@ -4482,7 +4558,7 @@
         <v>45271</v>
       </c>
       <c r="I44" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J44" s="32" t="s">
         <v>52</v>
@@ -4545,7 +4621,7 @@
         <v>45233</v>
       </c>
       <c r="I45" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J45" s="32" t="s">
         <v>52</v>
@@ -4608,7 +4684,7 @@
         <v>45253</v>
       </c>
       <c r="I46" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J46" s="32" t="s">
         <v>52</v>
@@ -4671,7 +4747,7 @@
         <v>45254</v>
       </c>
       <c r="I47" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J47" s="32" t="s">
         <v>52</v>
@@ -4734,7 +4810,7 @@
         <v>45271</v>
       </c>
       <c r="I48" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J48" s="32" t="s">
         <v>52</v>
@@ -4797,7 +4873,7 @@
         <v>45238</v>
       </c>
       <c r="I49" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J49" s="32" t="s">
         <v>52</v>
@@ -4860,7 +4936,7 @@
         <v>45238</v>
       </c>
       <c r="I50" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J50" s="32" t="s">
         <v>52</v>
@@ -4901,58 +4977,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15" t="s">
+    <row r="51" spans="1:25" s="108" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20" t="s">
+      <c r="E51" s="93"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="H51" s="32">
+      <c r="H51" s="97">
         <v>45260</v>
       </c>
-      <c r="I51" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="J51" s="32" t="s">
+      <c r="I51" s="96" t="s">
+        <v>240</v>
+      </c>
+      <c r="J51" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="K51" s="32" t="s">
+      <c r="K51" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="L51" s="36"/>
-      <c r="M51" s="36"/>
-      <c r="N51" s="36"/>
-      <c r="O51" s="54" t="s">
+      <c r="L51" s="98"/>
+      <c r="M51" s="98"/>
+      <c r="N51" s="98"/>
+      <c r="O51" s="114" t="s">
         <v>119</v>
       </c>
-      <c r="P51" s="32">
+      <c r="P51" s="97">
         <v>45302</v>
       </c>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="52"/>
-      <c r="S51" s="49" t="s">
+      <c r="Q51" s="92"/>
+      <c r="R51" s="100"/>
+      <c r="S51" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="T51" s="49"/>
-      <c r="U51" s="49"/>
-      <c r="V51" s="49"/>
-      <c r="W51" s="40" t="s">
+      <c r="T51" s="101"/>
+      <c r="U51" s="101"/>
+      <c r="V51" s="101"/>
+      <c r="W51" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="X51" s="55"/>
-      <c r="Y51" s="28">
+      <c r="X51" s="115"/>
+      <c r="Y51" s="107">
         <v>0</v>
       </c>
     </row>
@@ -4978,7 +5054,7 @@
         <v>45251</v>
       </c>
       <c r="I52" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J52" s="32" t="s">
         <v>52</v>
@@ -5041,7 +5117,7 @@
         <v>45265</v>
       </c>
       <c r="I53" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J53" s="32" t="s">
         <v>52</v>
@@ -5104,7 +5180,7 @@
         <v>45175</v>
       </c>
       <c r="I54" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J54" s="43" t="s">
         <v>46</v>
@@ -5145,7 +5221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="66" t="s">
         <v>126</v>
       </c>
@@ -5167,7 +5243,7 @@
         <v>45106</v>
       </c>
       <c r="I55" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J55" s="43" t="s">
         <v>46</v>
@@ -5218,7 +5294,7 @@
         <v>45309</v>
       </c>
       <c r="I56" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J56" s="43" t="s">
         <v>46</v>
@@ -5281,7 +5357,7 @@
         <v>45263</v>
       </c>
       <c r="I57" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J57" s="43" t="s">
         <v>46</v>
@@ -5322,7 +5398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="66" t="s">
         <v>130</v>
       </c>
@@ -5344,7 +5420,7 @@
         <v>45154</v>
       </c>
       <c r="I58" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J58" s="32" t="s">
         <v>131</v>
@@ -5373,7 +5449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="66" t="s">
         <v>132</v>
       </c>
@@ -5395,7 +5471,7 @@
         <v>45362</v>
       </c>
       <c r="I59" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J59" s="32" t="s">
         <v>131</v>
@@ -5424,7 +5500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="66" t="s">
         <v>133</v>
       </c>
@@ -5446,7 +5522,7 @@
         <v>45086</v>
       </c>
       <c r="I60" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J60" s="43" t="s">
         <v>36</v>
@@ -5497,7 +5573,7 @@
         <v>45247</v>
       </c>
       <c r="I61" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J61" s="43" t="s">
         <v>36</v>
@@ -5560,7 +5636,7 @@
         <v>45250</v>
       </c>
       <c r="I62" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J62" s="32" t="s">
         <v>137</v>
@@ -5601,7 +5677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="66" t="s">
         <v>139</v>
       </c>
@@ -5623,13 +5699,13 @@
         <v>45110</v>
       </c>
       <c r="I63" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J63" s="32" t="s">
         <v>140</v>
       </c>
       <c r="K63" s="32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L63" s="60"/>
       <c r="M63" s="60"/>
@@ -5637,26 +5713,38 @@
       <c r="O63" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="P63" s="32" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q63" s="15"/>
-      <c r="R63" s="52"/>
+      <c r="P63" s="32">
+        <v>45376</v>
+      </c>
+      <c r="Q63" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="R63" s="48">
+        <v>45376</v>
+      </c>
       <c r="S63" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="T63" s="49"/>
-      <c r="U63" s="49"/>
-      <c r="V63" s="49"/>
+        <v>29</v>
+      </c>
+      <c r="T63" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="U63" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="V63" s="53" t="s">
+        <v>270</v>
+      </c>
       <c r="W63" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X63" s="55"/>
-      <c r="Y63" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X63" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y63" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="66" t="s">
         <v>141</v>
       </c>
@@ -5678,7 +5766,7 @@
         <v>45096</v>
       </c>
       <c r="I64" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J64" s="32" t="s">
         <v>140</v>
@@ -5690,10 +5778,10 @@
       <c r="M64" s="60"/>
       <c r="N64" s="60"/>
       <c r="O64" s="54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P64" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q64" s="15"/>
       <c r="R64" s="52"/>
@@ -5711,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="66" t="s">
         <v>142</v>
       </c>
@@ -5731,7 +5819,7 @@
         <v>45218</v>
       </c>
       <c r="I65" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J65" s="32" t="s">
         <v>140</v>
@@ -5743,10 +5831,10 @@
       <c r="M65" s="60"/>
       <c r="N65" s="60"/>
       <c r="O65" s="60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P65" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q65" s="15"/>
       <c r="R65" s="52"/>
@@ -5764,7 +5852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="66" t="s">
         <v>143</v>
       </c>
@@ -5786,7 +5874,7 @@
         <v>45092</v>
       </c>
       <c r="I66" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J66" s="32" t="s">
         <v>140</v>
@@ -5799,7 +5887,7 @@
       <c r="N66" s="60"/>
       <c r="O66" s="60"/>
       <c r="P66" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q66" s="15"/>
       <c r="R66" s="52"/>
@@ -5817,7 +5905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="66" t="s">
         <v>144</v>
       </c>
@@ -5839,7 +5927,7 @@
         <v>45210</v>
       </c>
       <c r="I67" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J67" s="32" t="s">
         <v>140</v>
@@ -5852,7 +5940,7 @@
       <c r="N67" s="60"/>
       <c r="O67" s="60"/>
       <c r="P67" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q67" s="15"/>
       <c r="R67" s="52"/>
@@ -5892,7 +5980,7 @@
         <v>45210</v>
       </c>
       <c r="I68" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J68" s="32" t="s">
         <v>140</v>
@@ -5933,7 +6021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="66" t="s">
         <v>146</v>
       </c>
@@ -5955,7 +6043,7 @@
         <v>45096</v>
       </c>
       <c r="I69" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J69" s="32" t="s">
         <v>140</v>
@@ -5968,7 +6056,7 @@
       <c r="N69" s="60"/>
       <c r="O69" s="60"/>
       <c r="P69" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q69" s="15"/>
       <c r="R69" s="52"/>
@@ -5986,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="66" t="s">
         <v>147</v>
       </c>
@@ -6008,7 +6096,7 @@
         <v>45292</v>
       </c>
       <c r="I70" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J70" s="32" t="s">
         <v>140</v>
@@ -6020,10 +6108,10 @@
       <c r="M70" s="60"/>
       <c r="N70" s="60"/>
       <c r="O70" s="54" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P70" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q70" s="15"/>
       <c r="R70" s="52"/>
@@ -6041,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="66" t="s">
         <v>148</v>
       </c>
@@ -6063,7 +6151,7 @@
         <v>45096</v>
       </c>
       <c r="I71" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J71" s="32" t="s">
         <v>140</v>
@@ -6076,7 +6164,7 @@
       <c r="N71" s="60"/>
       <c r="O71" s="60"/>
       <c r="P71" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q71" s="15"/>
       <c r="R71" s="52"/>
@@ -6094,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="66" t="s">
         <v>149</v>
       </c>
@@ -6116,7 +6204,7 @@
         <v>45345</v>
       </c>
       <c r="I72" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J72" s="32" t="s">
         <v>69</v>
@@ -6131,7 +6219,7 @@
         <v>27</v>
       </c>
       <c r="P72" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q72" s="15"/>
       <c r="R72" s="52"/>
@@ -6149,7 +6237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="66" t="s">
         <v>150</v>
       </c>
@@ -6171,7 +6259,7 @@
         <v>45209</v>
       </c>
       <c r="I73" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J73" s="32" t="s">
         <v>69</v>
@@ -6183,10 +6271,10 @@
       <c r="M73" s="60"/>
       <c r="N73" s="60"/>
       <c r="O73" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P73" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q73" s="15"/>
       <c r="R73" s="52"/>
@@ -6204,7 +6292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="66" t="s">
         <v>151</v>
       </c>
@@ -6226,7 +6314,7 @@
         <v>45170</v>
       </c>
       <c r="I74" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J74" s="32" t="s">
         <v>69</v>
@@ -6238,10 +6326,10 @@
       <c r="M74" s="60"/>
       <c r="N74" s="60"/>
       <c r="O74" s="54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P74" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q74" s="15"/>
       <c r="R74" s="52"/>
@@ -6259,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="66" t="s">
         <v>152</v>
       </c>
@@ -6281,7 +6369,7 @@
         <v>45247</v>
       </c>
       <c r="I75" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J75" s="32" t="s">
         <v>69</v>
@@ -6293,10 +6381,10 @@
       <c r="M75" s="60"/>
       <c r="N75" s="60"/>
       <c r="O75" s="54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P75" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q75" s="15"/>
       <c r="R75" s="52"/>
@@ -6336,7 +6424,7 @@
         <v>45241</v>
       </c>
       <c r="I76" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J76" s="32" t="s">
         <v>69</v>
@@ -6377,7 +6465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="66" t="s">
         <v>154</v>
       </c>
@@ -6399,7 +6487,7 @@
         <v>45248</v>
       </c>
       <c r="I77" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J77" s="32" t="s">
         <v>69</v>
@@ -6411,10 +6499,10 @@
       <c r="M77" s="60"/>
       <c r="N77" s="60"/>
       <c r="O77" s="54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P77" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q77" s="15"/>
       <c r="R77" s="52"/>
@@ -6432,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="66" t="s">
         <v>155</v>
       </c>
@@ -6454,7 +6542,7 @@
         <v>45210</v>
       </c>
       <c r="I78" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J78" s="32" t="s">
         <v>69</v>
@@ -6466,10 +6554,10 @@
       <c r="M78" s="60"/>
       <c r="N78" s="60"/>
       <c r="O78" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P78" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="52"/>
@@ -6487,7 +6575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="66" t="s">
         <v>156</v>
       </c>
@@ -6509,7 +6597,7 @@
         <v>45261</v>
       </c>
       <c r="I79" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J79" s="32" t="s">
         <v>69</v>
@@ -6521,10 +6609,10 @@
       <c r="M79" s="60"/>
       <c r="N79" s="60"/>
       <c r="O79" s="54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P79" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q79" s="15"/>
       <c r="R79" s="52"/>
@@ -6542,70 +6630,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" s="102" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="89" t="s">
+    <row r="80" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="90" t="s">
+      <c r="B80" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C80" s="91" t="s">
+      <c r="C80" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D80" s="92" t="s">
+      <c r="D80" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E80" s="91"/>
-      <c r="F80" s="91"/>
-      <c r="G80" s="91" t="s">
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H80" s="93">
+      <c r="H80" s="32">
         <v>45175</v>
       </c>
-      <c r="I80" s="94" t="s">
-        <v>246</v>
-      </c>
-      <c r="J80" s="93" t="s">
+      <c r="I80" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="J80" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="K80" s="93" t="s">
+      <c r="K80" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L80" s="95"/>
-      <c r="M80" s="95"/>
-      <c r="N80" s="95"/>
-      <c r="O80" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="P80" s="97">
+      <c r="L80" s="60"/>
+      <c r="M80" s="60"/>
+      <c r="N80" s="60"/>
+      <c r="O80" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="P80" s="84">
         <v>45261</v>
       </c>
-      <c r="Q80" s="90" t="s">
+      <c r="Q80" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="R80" s="98">
+      <c r="R80" s="52">
         <v>45261</v>
       </c>
-      <c r="S80" s="99" t="s">
+      <c r="S80" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="T80" s="99" t="s">
+      <c r="T80" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="U80" s="99"/>
-      <c r="V80" s="99"/>
-      <c r="W80" s="100" t="s">
+      <c r="U80" s="49"/>
+      <c r="V80" s="49"/>
+      <c r="W80" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X80" s="101" t="s">
+      <c r="X80" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="Y80" s="101">
+      <c r="Y80" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="71" t="s">
         <v>160</v>
       </c>
@@ -6627,7 +6715,7 @@
         <v>45253</v>
       </c>
       <c r="I81" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J81" s="32" t="s">
         <v>161</v>
@@ -6642,7 +6730,7 @@
         <v>27</v>
       </c>
       <c r="P81" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q81" s="15"/>
       <c r="R81" s="52"/>
@@ -6682,7 +6770,7 @@
         <v>45253</v>
       </c>
       <c r="I82" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J82" s="44" t="s">
         <v>44</v>
@@ -6745,7 +6833,7 @@
         <v>45244</v>
       </c>
       <c r="I83" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J83" s="44" t="s">
         <v>44</v>
@@ -6762,8 +6850,8 @@
       <c r="P83" s="32">
         <v>45274</v>
       </c>
-      <c r="Q83" s="67" t="s">
-        <v>164</v>
+      <c r="Q83" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="R83" s="52">
         <v>45274</v>
@@ -6788,7 +6876,7 @@
     </row>
     <row r="84" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B84" s="15" t="s">
         <v>33</v>
@@ -6808,7 +6896,7 @@
         <v>45253</v>
       </c>
       <c r="I84" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J84" s="32" t="s">
         <v>137</v>
@@ -6820,12 +6908,12 @@
       <c r="M84" s="36"/>
       <c r="N84" s="36"/>
       <c r="O84" s="54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P84" s="32">
         <v>45279</v>
       </c>
-      <c r="Q84" s="4" t="s">
+      <c r="Q84" s="15" t="s">
         <v>30</v>
       </c>
       <c r="R84" s="52">
@@ -6851,7 +6939,7 @@
     </row>
     <row r="85" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B85" s="15" t="s">
         <v>33</v>
@@ -6871,7 +6959,7 @@
         <v>45259</v>
       </c>
       <c r="I85" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J85" s="72" t="s">
         <v>52</v>
@@ -6914,7 +7002,7 @@
     </row>
     <row r="86" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>33</v>
@@ -6934,7 +7022,7 @@
         <v>45289</v>
       </c>
       <c r="I86" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J86" s="32" t="s">
         <v>52</v>
@@ -6977,7 +7065,7 @@
     </row>
     <row r="87" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>33</v>
@@ -6997,10 +7085,10 @@
         <v>45296</v>
       </c>
       <c r="I87" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J87" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K87" s="32" t="s">
         <v>25</v>
@@ -7040,7 +7128,7 @@
     </row>
     <row r="88" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>33</v>
@@ -7060,7 +7148,7 @@
         <v>45275</v>
       </c>
       <c r="I88" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J88" s="43" t="s">
         <v>46</v>
@@ -7101,15 +7189,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B89" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D89" s="20" t="s">
         <v>24</v>
@@ -7123,7 +7211,7 @@
         <v>45214</v>
       </c>
       <c r="I89" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J89" s="32" t="s">
         <v>39</v>
@@ -7138,7 +7226,7 @@
         <v>71</v>
       </c>
       <c r="P89" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q89" s="15"/>
       <c r="R89" s="52"/>
@@ -7158,13 +7246,13 @@
     </row>
     <row r="90" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B90" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D90" s="31" t="s">
         <v>24</v>
@@ -7178,7 +7266,7 @@
         <v>45267</v>
       </c>
       <c r="I90" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J90" s="32" t="s">
         <v>39</v>
@@ -7219,15 +7307,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B91" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D91" s="20" t="s">
         <v>24</v>
@@ -7241,7 +7329,7 @@
         <v>45229</v>
       </c>
       <c r="I91" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J91" s="32" t="s">
         <v>39</v>
@@ -7256,7 +7344,7 @@
         <v>71</v>
       </c>
       <c r="P91" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q91" s="15"/>
       <c r="R91" s="52"/>
@@ -7274,15 +7362,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B92" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D92" s="76" t="s">
         <v>24</v>
@@ -7296,7 +7384,7 @@
         <v>45216</v>
       </c>
       <c r="I92" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J92" s="32" t="s">
         <v>39</v>
@@ -7311,7 +7399,7 @@
         <v>27</v>
       </c>
       <c r="P92" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q92" s="15"/>
       <c r="R92" s="52"/>
@@ -7329,15 +7417,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B93" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C93" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D93" s="20" t="s">
         <v>35</v>
@@ -7351,7 +7439,7 @@
         <v>45267</v>
       </c>
       <c r="I93" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J93" s="32" t="s">
         <v>39</v>
@@ -7366,7 +7454,7 @@
         <v>71</v>
       </c>
       <c r="P93" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q93" s="15"/>
       <c r="R93" s="52"/>
@@ -7384,7 +7472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>132</v>
       </c>
@@ -7392,7 +7480,7 @@
         <v>33</v>
       </c>
       <c r="C94" s="77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D94" s="20" t="s">
         <v>35</v>
@@ -7406,10 +7494,10 @@
         <v>45306</v>
       </c>
       <c r="I94" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J94" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K94" s="32" t="s">
         <v>30</v>
@@ -7424,26 +7512,26 @@
       <c r="S94" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="T94" s="73"/>
+      <c r="T94" s="49"/>
       <c r="U94" s="73"/>
       <c r="V94" s="73"/>
       <c r="W94" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X94" s="55"/>
-      <c r="Y94" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X94" s="41"/>
+      <c r="Y94" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B95" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C95" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D95" s="20" t="s">
         <v>35</v>
@@ -7457,7 +7545,7 @@
         <v>45260</v>
       </c>
       <c r="I95" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J95" s="32" t="s">
         <v>39</v>
@@ -7472,7 +7560,7 @@
         <v>71</v>
       </c>
       <c r="P95" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q95" s="15"/>
       <c r="R95" s="52"/>
@@ -7490,15 +7578,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C96" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D96" s="20" t="s">
         <v>35</v>
@@ -7512,7 +7600,7 @@
         <v>45278</v>
       </c>
       <c r="I96" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J96" s="32" t="s">
         <v>39</v>
@@ -7527,7 +7615,7 @@
         <v>71</v>
       </c>
       <c r="P96" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q96" s="15"/>
       <c r="R96" s="52"/>
@@ -7545,15 +7633,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B97" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C97" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D97" s="20" t="s">
         <v>35</v>
@@ -7567,7 +7655,7 @@
         <v>45275</v>
       </c>
       <c r="I97" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J97" s="32" t="s">
         <v>39</v>
@@ -7582,7 +7670,7 @@
         <v>71</v>
       </c>
       <c r="P97" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q97" s="15"/>
       <c r="R97" s="52"/>
@@ -7602,13 +7690,13 @@
     </row>
     <row r="98" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C98" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D98" s="31" t="s">
         <v>24</v>
@@ -7622,7 +7710,7 @@
         <v>45310</v>
       </c>
       <c r="I98" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J98" s="32" t="s">
         <v>140</v>
@@ -7665,7 +7753,7 @@
     </row>
     <row r="99" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B99" s="15" t="s">
         <v>33</v>
@@ -7685,7 +7773,7 @@
         <v>45320</v>
       </c>
       <c r="I99" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J99" s="32" t="s">
         <v>52</v>
@@ -7726,9 +7814,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:25" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B100" s="15" t="s">
         <v>33</v>
@@ -7748,7 +7836,7 @@
         <v>45317</v>
       </c>
       <c r="I100" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J100" s="32" t="s">
         <v>52</v>
@@ -7760,7 +7848,7 @@
       <c r="M100" s="36"/>
       <c r="N100" s="36"/>
       <c r="O100" s="47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P100" s="46"/>
       <c r="Q100" s="15"/>
@@ -7779,9 +7867,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B101" s="15" t="s">
         <v>33</v>
@@ -7801,7 +7889,7 @@
         <v>45243</v>
       </c>
       <c r="I101" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J101" s="32" t="s">
         <v>39</v>
@@ -7816,7 +7904,7 @@
         <v>27</v>
       </c>
       <c r="P101" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q101" s="15"/>
       <c r="R101" s="52"/>
@@ -7836,7 +7924,7 @@
     </row>
     <row r="102" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>33</v>
@@ -7856,7 +7944,7 @@
         <v>45262</v>
       </c>
       <c r="I102" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J102" s="32" t="s">
         <v>52</v>
@@ -7897,9 +7985,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>33</v>
@@ -7919,7 +8007,7 @@
         <v>45267</v>
       </c>
       <c r="I103" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J103" s="32" t="s">
         <v>39</v>
@@ -7931,10 +8019,10 @@
       <c r="M103" s="60"/>
       <c r="N103" s="60"/>
       <c r="O103" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P103" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q103" s="15"/>
       <c r="R103" s="52"/>
@@ -7952,9 +8040,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>33</v>
@@ -7974,7 +8062,7 @@
         <v>45267</v>
       </c>
       <c r="I104" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J104" s="32" t="s">
         <v>39</v>
@@ -7989,7 +8077,7 @@
         <v>27</v>
       </c>
       <c r="P104" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q104" s="15"/>
       <c r="R104" s="52"/>
@@ -8007,9 +8095,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B105" s="15" t="s">
         <v>33</v>
@@ -8029,7 +8117,7 @@
         <v>45267</v>
       </c>
       <c r="I105" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J105" s="32" t="s">
         <v>39</v>
@@ -8044,7 +8132,7 @@
         <v>27</v>
       </c>
       <c r="P105" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q105" s="15"/>
       <c r="R105" s="52"/>
@@ -8062,9 +8150,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B106" s="15" t="s">
         <v>33</v>
@@ -8084,7 +8172,7 @@
         <v>45268</v>
       </c>
       <c r="I106" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J106" s="32" t="s">
         <v>39</v>
@@ -8099,7 +8187,7 @@
         <v>27</v>
       </c>
       <c r="P106" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q106" s="15"/>
       <c r="R106" s="52"/>
@@ -8117,9 +8205,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>33</v>
@@ -8139,7 +8227,7 @@
         <v>45313</v>
       </c>
       <c r="I107" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J107" s="32" t="s">
         <v>39</v>
@@ -8151,10 +8239,10 @@
       <c r="M107" s="60"/>
       <c r="N107" s="60"/>
       <c r="O107" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P107" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q107" s="15"/>
       <c r="R107" s="52"/>
@@ -8172,9 +8260,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>33</v>
@@ -8194,7 +8282,7 @@
         <v>45313</v>
       </c>
       <c r="I108" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J108" s="32" t="s">
         <v>39</v>
@@ -8206,10 +8294,10 @@
       <c r="M108" s="60"/>
       <c r="N108" s="60"/>
       <c r="O108" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P108" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q108" s="15"/>
       <c r="R108" s="52"/>
@@ -8227,9 +8315,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B109" s="15" t="s">
         <v>33</v>
@@ -8249,7 +8337,7 @@
         <v>45313</v>
       </c>
       <c r="I109" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J109" s="32" t="s">
         <v>39</v>
@@ -8261,10 +8349,10 @@
       <c r="M109" s="60"/>
       <c r="N109" s="60"/>
       <c r="O109" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P109" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q109" s="15"/>
       <c r="R109" s="52"/>
@@ -8282,9 +8370,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B110" s="15" t="s">
         <v>33</v>
@@ -8304,7 +8392,7 @@
         <v>45293</v>
       </c>
       <c r="I110" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J110" s="32" t="s">
         <v>39</v>
@@ -8316,10 +8404,10 @@
       <c r="M110" s="60"/>
       <c r="N110" s="60"/>
       <c r="O110" s="54" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P110" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q110" s="15"/>
       <c r="R110" s="52"/>
@@ -8337,9 +8425,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B111" s="15" t="s">
         <v>33</v>
@@ -8359,7 +8447,7 @@
         <v>45313</v>
       </c>
       <c r="I111" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J111" s="32" t="s">
         <v>39</v>
@@ -8374,7 +8462,7 @@
         <v>80</v>
       </c>
       <c r="P111" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q111" s="15"/>
       <c r="R111" s="52"/>
@@ -8394,13 +8482,13 @@
     </row>
     <row r="112" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B112" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C112" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D112" s="31" t="s">
         <v>24</v>
@@ -8414,7 +8502,7 @@
         <v>45293</v>
       </c>
       <c r="I112" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J112" s="43" t="s">
         <v>46</v>
@@ -8435,7 +8523,7 @@
       <c r="R112" s="48">
         <v>45359</v>
       </c>
-      <c r="S112" s="87" t="s">
+      <c r="S112" s="83" t="s">
         <v>29</v>
       </c>
       <c r="T112" s="49" t="s">
@@ -8455,7 +8543,7 @@
     </row>
     <row r="113" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B113" s="15" t="s">
         <v>33</v>
@@ -8475,7 +8563,7 @@
         <v>45299</v>
       </c>
       <c r="I113" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J113" s="32" t="s">
         <v>39</v>
@@ -8514,9 +8602,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>33</v>
@@ -8533,10 +8621,10 @@
         <v>25</v>
       </c>
       <c r="H114" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I114" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J114" s="32" t="s">
         <v>69</v>
@@ -8548,10 +8636,10 @@
       <c r="M114" s="36"/>
       <c r="N114" s="36"/>
       <c r="O114" s="54" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P114" s="69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q114" s="58" t="s">
         <v>30</v>
@@ -8573,9 +8661,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B115" s="15" t="s">
         <v>33</v>
@@ -8595,7 +8683,7 @@
         <v>45019</v>
       </c>
       <c r="I115" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J115" s="32" t="s">
         <v>52</v>
@@ -8626,9 +8714,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:25" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B116" s="15" t="s">
         <v>33</v>
@@ -8648,7 +8736,7 @@
         <v>43925</v>
       </c>
       <c r="I116" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J116" s="32" t="s">
         <v>39</v>
@@ -8660,10 +8748,10 @@
       <c r="M116" s="36"/>
       <c r="N116" s="36"/>
       <c r="O116" s="60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P116" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q116" s="15"/>
       <c r="R116" s="52"/>
@@ -8681,15 +8769,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C117" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D117" s="78" t="s">
         <v>35</v>
@@ -8703,7 +8791,7 @@
         <v>45317</v>
       </c>
       <c r="I117" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J117" s="32" t="s">
         <v>39</v>
@@ -8718,7 +8806,7 @@
         <v>71</v>
       </c>
       <c r="P117" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q117" s="15"/>
       <c r="R117" s="52"/>
@@ -8736,15 +8824,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C118" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D118" s="78" t="s">
         <v>35</v>
@@ -8758,7 +8846,7 @@
         <v>45316</v>
       </c>
       <c r="I118" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J118" s="32" t="s">
         <v>39</v>
@@ -8773,7 +8861,7 @@
         <v>71</v>
       </c>
       <c r="P118" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q118" s="15"/>
       <c r="R118" s="52"/>
@@ -8791,9 +8879,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B119" s="15" t="s">
         <v>33</v>
@@ -8813,7 +8901,7 @@
         <v>45161</v>
       </c>
       <c r="I119" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J119" s="32" t="s">
         <v>39</v>
@@ -8846,15 +8934,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B120" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C120" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D120" s="78" t="s">
         <v>35</v>
@@ -8868,7 +8956,7 @@
         <v>45317</v>
       </c>
       <c r="I120" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J120" s="32" t="s">
         <v>39</v>
@@ -8883,7 +8971,7 @@
         <v>71</v>
       </c>
       <c r="P120" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q120" s="15"/>
       <c r="R120" s="52"/>
@@ -8903,13 +8991,13 @@
     </row>
     <row r="121" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B121" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C121" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D121" s="31" t="s">
         <v>24</v>
@@ -8923,7 +9011,7 @@
         <v>45317</v>
       </c>
       <c r="I121" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J121" s="32" t="s">
         <v>39</v>
@@ -8962,64 +9050,76 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="B122" s="15" t="s">
+    <row r="122" spans="1:25" s="108" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="92" t="s">
+        <v>205</v>
+      </c>
+      <c r="B122" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C122" s="20" t="s">
+      <c r="C122" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="D122" s="78" t="s">
+      <c r="D122" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="E122" s="20"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="20" t="s">
+      <c r="E122" s="93"/>
+      <c r="F122" s="93"/>
+      <c r="G122" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="H122" s="32">
+      <c r="H122" s="97">
         <v>45325</v>
       </c>
-      <c r="I122" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="J122" s="32" t="s">
+      <c r="I122" s="96" t="s">
+        <v>240</v>
+      </c>
+      <c r="J122" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="K122" s="32" t="s">
+      <c r="K122" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="L122" s="36"/>
-      <c r="M122" s="36"/>
-      <c r="N122" s="36"/>
-      <c r="O122" s="36" t="s">
+      <c r="L122" s="98"/>
+      <c r="M122" s="98"/>
+      <c r="N122" s="98"/>
+      <c r="O122" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="P122" s="32">
+      <c r="P122" s="97">
         <v>45364</v>
       </c>
-      <c r="Q122" s="58"/>
-      <c r="R122" s="52"/>
-      <c r="S122" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="T122" s="73"/>
-      <c r="U122" s="73"/>
-      <c r="V122" s="73"/>
-      <c r="W122" s="40" t="s">
+      <c r="Q122" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="X122" s="55"/>
-      <c r="Y122" s="28">
-        <v>0</v>
+      <c r="R122" s="100">
+        <v>45364</v>
+      </c>
+      <c r="S122" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="T122" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="U122" s="103" t="s">
+        <v>265</v>
+      </c>
+      <c r="V122" s="104" t="s">
+        <v>266</v>
+      </c>
+      <c r="W122" s="105" t="s">
+        <v>30</v>
+      </c>
+      <c r="X122" s="116" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y122" s="116">
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B123" s="15" t="s">
         <v>33</v>
@@ -9039,7 +9139,7 @@
         <v>45320</v>
       </c>
       <c r="I123" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J123" s="32" t="s">
         <v>52</v>
@@ -9060,7 +9160,7 @@
       <c r="R123" s="48">
         <v>45352</v>
       </c>
-      <c r="S123" s="87" t="s">
+      <c r="S123" s="83" t="s">
         <v>29</v>
       </c>
       <c r="T123" s="49" t="s">
@@ -9078,9 +9178,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="67" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B124" s="15" t="s">
         <v>33</v>
@@ -9100,7 +9200,7 @@
         <v>45161</v>
       </c>
       <c r="I124" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J124" s="32" t="s">
         <v>140</v>
@@ -9112,10 +9212,10 @@
       <c r="M124" s="60"/>
       <c r="N124" s="60"/>
       <c r="O124" s="54" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P124" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q124" s="15"/>
       <c r="R124" s="52"/>
@@ -9133,9 +9233,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B125" s="15" t="s">
         <v>33</v>
@@ -9155,7 +9255,7 @@
         <v>45161</v>
       </c>
       <c r="I125" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J125" s="32" t="s">
         <v>39</v>
@@ -9170,7 +9270,7 @@
         <v>27</v>
       </c>
       <c r="P125" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q125" s="15"/>
       <c r="R125" s="52"/>
@@ -9188,9 +9288,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B126" s="15" t="s">
         <v>33</v>
@@ -9210,7 +9310,7 @@
         <v>45329</v>
       </c>
       <c r="I126" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J126" s="32" t="s">
         <v>39</v>
@@ -9222,10 +9322,10 @@
       <c r="M126" s="60"/>
       <c r="N126" s="60"/>
       <c r="O126" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P126" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q126" s="15"/>
       <c r="R126" s="52"/>
@@ -9245,7 +9345,7 @@
     </row>
     <row r="127" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B127" s="15" t="s">
         <v>33</v>
@@ -9265,7 +9365,7 @@
         <v>45325</v>
       </c>
       <c r="I127" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J127" s="32" t="s">
         <v>52</v>
@@ -9304,68 +9404,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:25" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="79" t="s">
-        <v>211</v>
-      </c>
-      <c r="B128" s="15" t="s">
+    <row r="128" spans="1:25" s="108" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="91" t="s">
+        <v>210</v>
+      </c>
+      <c r="B128" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C128" s="20" t="s">
+      <c r="C128" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="D128" s="80" t="s">
+      <c r="D128" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="E128" s="20"/>
-      <c r="F128" s="20"/>
-      <c r="G128" s="20" t="s">
+      <c r="E128" s="93"/>
+      <c r="F128" s="93"/>
+      <c r="G128" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="H128" s="82">
+      <c r="H128" s="95">
         <v>45325</v>
       </c>
-      <c r="I128" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="J128" s="32" t="s">
+      <c r="I128" s="96" t="s">
+        <v>240</v>
+      </c>
+      <c r="J128" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="K128" s="32" t="s">
+      <c r="K128" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="L128" s="32"/>
-      <c r="M128" s="32"/>
-      <c r="N128" s="36"/>
-      <c r="O128" s="36" t="s">
+      <c r="L128" s="97"/>
+      <c r="M128" s="97"/>
+      <c r="N128" s="98"/>
+      <c r="O128" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="P128" s="82">
+      <c r="P128" s="95">
         <v>45359</v>
       </c>
-      <c r="Q128" s="58" t="s">
+      <c r="Q128" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="R128" s="52">
+      <c r="R128" s="100">
         <v>45342</v>
       </c>
-      <c r="S128" s="49" t="s">
+      <c r="S128" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="T128" s="83"/>
-      <c r="U128" s="75"/>
-      <c r="V128" s="73"/>
-      <c r="W128" s="40" t="s">
+      <c r="T128" s="102"/>
+      <c r="U128" s="103"/>
+      <c r="V128" s="104"/>
+      <c r="W128" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="X128" s="84"/>
-      <c r="Y128" s="28">
+      <c r="X128" s="106"/>
+      <c r="Y128" s="107">
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:25" s="26" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B129" s="15" t="s">
         <v>33</v>
@@ -9377,7 +9477,7 @@
         <v>24</v>
       </c>
       <c r="E129" s="20"/>
-      <c r="F129" s="81"/>
+      <c r="F129" s="79"/>
       <c r="G129" s="20" t="s">
         <v>25</v>
       </c>
@@ -9385,7 +9485,7 @@
         <v>43925</v>
       </c>
       <c r="I129" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J129" s="32" t="s">
         <v>39</v>
@@ -9402,10 +9502,10 @@
       <c r="P129" s="32">
         <v>45344</v>
       </c>
-      <c r="Q129" s="85" t="s">
-        <v>212</v>
-      </c>
-      <c r="R129" s="86">
+      <c r="Q129" s="81" t="s">
+        <v>211</v>
+      </c>
+      <c r="R129" s="82">
         <v>45351</v>
       </c>
       <c r="S129" s="49" t="s">
@@ -9414,8 +9514,8 @@
       <c r="T129" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="U129" s="83"/>
-      <c r="V129" s="83"/>
+      <c r="U129" s="80"/>
+      <c r="V129" s="80"/>
       <c r="W129" s="40" t="s">
         <v>30</v>
       </c>
@@ -9428,7 +9528,7 @@
     </row>
     <row r="130" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B130" s="15" t="s">
         <v>33</v>
@@ -9448,7 +9548,7 @@
         <v>45333</v>
       </c>
       <c r="I130" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J130" s="32" t="s">
         <v>52</v>
@@ -9489,7 +9589,7 @@
     </row>
     <row r="131" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B131" s="15" t="s">
         <v>33</v>
@@ -9509,7 +9609,7 @@
         <v>45325</v>
       </c>
       <c r="I131" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J131" s="32" t="s">
         <v>52</v>
@@ -9548,9 +9648,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B132" s="15" t="s">
         <v>33</v>
@@ -9570,10 +9670,10 @@
         <v>45106</v>
       </c>
       <c r="I132" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J132" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K132" s="32" t="s">
         <v>25</v>
@@ -9582,30 +9682,42 @@
       <c r="M132" s="60"/>
       <c r="N132" s="60"/>
       <c r="O132" s="60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P132" s="32">
         <v>45366</v>
       </c>
-      <c r="Q132" s="15"/>
-      <c r="R132" s="52"/>
+      <c r="Q132" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="R132" s="48">
+        <v>45366</v>
+      </c>
       <c r="S132" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="T132" s="73"/>
-      <c r="U132" s="73"/>
-      <c r="V132" s="73"/>
+        <v>29</v>
+      </c>
+      <c r="T132" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="U132" s="75" t="s">
+        <v>267</v>
+      </c>
+      <c r="V132" s="73" t="s">
+        <v>268</v>
+      </c>
       <c r="W132" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="X132" s="55"/>
-      <c r="Y132" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X132" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y132" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B133" s="15" t="s">
         <v>33</v>
@@ -9625,10 +9737,10 @@
         <v>45336</v>
       </c>
       <c r="I133" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="J133" s="32" t="s">
         <v>249</v>
-      </c>
-      <c r="J133" s="32" t="s">
-        <v>250</v>
       </c>
       <c r="K133" s="32" t="s">
         <v>30</v>
@@ -9638,7 +9750,7 @@
       <c r="N133" s="22"/>
       <c r="O133" s="60"/>
       <c r="P133" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q133" s="4"/>
       <c r="R133" s="7"/>
@@ -9656,9 +9768,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>33</v>
@@ -9678,10 +9790,10 @@
         <v>45327</v>
       </c>
       <c r="I134" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="J134" s="32" t="s">
         <v>249</v>
-      </c>
-      <c r="J134" s="32" t="s">
-        <v>250</v>
       </c>
       <c r="K134" s="32" t="s">
         <v>30</v>
@@ -9691,7 +9803,7 @@
       <c r="N134" s="22"/>
       <c r="O134" s="60"/>
       <c r="P134" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q134" s="4"/>
       <c r="R134" s="7"/>
@@ -9709,9 +9821,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>33</v>
@@ -9731,10 +9843,10 @@
         <v>45138</v>
       </c>
       <c r="I135" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="J135" s="32" t="s">
         <v>249</v>
-      </c>
-      <c r="J135" s="32" t="s">
-        <v>250</v>
       </c>
       <c r="K135" s="32" t="s">
         <v>30</v>
@@ -9744,7 +9856,7 @@
       <c r="N135" s="22"/>
       <c r="O135" s="60"/>
       <c r="P135" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q135" s="4"/>
       <c r="R135" s="7"/>
@@ -9762,9 +9874,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B136" s="15" t="s">
         <v>33</v>
@@ -9784,7 +9896,7 @@
         <v>45292</v>
       </c>
       <c r="I136" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J136" s="32" t="s">
         <v>69</v>
@@ -9797,7 +9909,7 @@
       <c r="N136" s="22"/>
       <c r="O136" s="60"/>
       <c r="P136" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q136" s="4"/>
       <c r="R136" s="7"/>
@@ -9815,59 +9927,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="4"/>
-      <c r="B137" s="4"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="20"/>
-      <c r="F137" s="20"/>
-      <c r="G137" s="20"/>
-      <c r="H137" s="5"/>
-      <c r="I137" s="5"/>
-      <c r="J137" s="5"/>
-      <c r="K137" s="5"/>
-      <c r="L137" s="22"/>
-      <c r="M137" s="22"/>
-      <c r="N137" s="22"/>
-      <c r="O137" s="22"/>
-      <c r="P137" s="5"/>
-      <c r="Q137" s="4"/>
-      <c r="R137" s="7"/>
-      <c r="S137" s="21"/>
-      <c r="T137" s="21"/>
-      <c r="U137" s="21"/>
-      <c r="V137" s="21"/>
-      <c r="W137" s="4"/>
-      <c r="X137" s="15"/>
-      <c r="Y137" s="28"/>
-    </row>
-    <row r="138" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="4"/>
-      <c r="B138" s="4"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
+    <row r="137" spans="1:25" s="108" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="B137" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="C137" s="93" t="s">
+        <v>34</v>
+      </c>
+      <c r="D137" s="109"/>
+      <c r="E137" s="93"/>
+      <c r="F137" s="93"/>
+      <c r="G137" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="H137" s="97">
+        <v>45369</v>
+      </c>
+      <c r="I137" s="96" t="s">
+        <v>240</v>
+      </c>
+      <c r="J137" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="K137" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="L137" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="M137" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="N137" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="O137" s="110" t="s">
+        <v>264</v>
+      </c>
+      <c r="P137" s="97" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q137" s="111"/>
+      <c r="R137" s="112"/>
+      <c r="S137" s="101" t="s">
+        <v>61</v>
+      </c>
+      <c r="T137" s="113"/>
+      <c r="U137" s="113"/>
+      <c r="V137" s="113"/>
+      <c r="W137" s="111"/>
+      <c r="X137" s="92"/>
+      <c r="Y137" s="116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:25" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B138" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C138" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D138" s="78"/>
       <c r="E138" s="20"/>
       <c r="F138" s="20"/>
-      <c r="G138" s="20"/>
-      <c r="H138" s="5"/>
-      <c r="I138" s="5"/>
-      <c r="J138" s="5"/>
-      <c r="K138" s="5"/>
-      <c r="L138" s="22"/>
-      <c r="M138" s="22"/>
-      <c r="N138" s="22"/>
-      <c r="O138" s="22"/>
-      <c r="P138" s="5"/>
-      <c r="Q138" s="4"/>
-      <c r="R138" s="7"/>
-      <c r="S138" s="21"/>
-      <c r="T138" s="21"/>
-      <c r="U138" s="21"/>
-      <c r="V138" s="21"/>
-      <c r="W138" s="4"/>
-      <c r="X138" s="15"/>
-      <c r="Y138" s="28"/>
+      <c r="G138" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H138" s="32">
+        <v>45301</v>
+      </c>
+      <c r="I138" s="46" t="s">
+        <v>272</v>
+      </c>
+      <c r="J138" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="K138" s="32">
+        <v>45371</v>
+      </c>
+      <c r="L138" s="60"/>
+      <c r="M138" s="60"/>
+      <c r="N138" s="60"/>
+      <c r="O138" s="60"/>
+      <c r="P138" s="32">
+        <v>45371</v>
+      </c>
+      <c r="Q138" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="R138" s="48">
+        <v>45371</v>
+      </c>
+      <c r="S138" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="T138" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="U138" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="V138" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="W138" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="X138" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y138" s="41">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4"/>
@@ -24632,13 +24810,7 @@
       <c r="Z669" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z136" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
-    <filterColumn colId="18">
-      <filters>
-        <filter val="REALIZADO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Z138" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -24662,13 +24834,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -25140,7 +25312,7 @@
       </c>
       <c r="B36" s="1" t="e">
         <f>Dados_Onboarding!P30-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C36" s="1">
         <f>Dados_Onboarding!R30-Dados_Onboarding!H30</f>
@@ -25630,11 +25802,11 @@
       </c>
       <c r="B71" s="1" t="e">
         <f>Dados_Onboarding!P63-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C71" s="1">
         <f>Dados_Onboarding!R63-Dados_Onboarding!H63</f>
-        <v>-45110</v>
+        <v>266</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -26502,7 +26674,7 @@
       </c>
       <c r="C133" s="1">
         <f>Dados_Onboarding!R122-Dados_Onboarding!H122</f>
-        <v>-45325</v>
+        <v>39</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -26656,7 +26828,7 @@
       </c>
       <c r="C144" s="1">
         <f>Dados_Onboarding!R132-Dados_Onboarding!H132</f>
-        <v>-45106</v>
+        <v>260</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -26722,11 +26894,11 @@
       </c>
       <c r="B149" s="1" t="e">
         <f>Dados_Onboarding!P137-Dados_Onboarding!#REF!</f>
-        <v>#REF!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C149" s="1">
         <f>Dados_Onboarding!R137-Dados_Onboarding!H137</f>
-        <v>0</v>
+        <v>-45369</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -26740,7 +26912,7 @@
       </c>
       <c r="C150" s="1">
         <f>Dados_Onboarding!R138-Dados_Onboarding!H138</f>
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -34183,14 +34355,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1" s="88"/>
+      <c r="A1" s="85" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="85"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="11" t="e">
         <f>AVERAGEIF('Base SLA'!A3:A690,"&gt;0")</f>
@@ -34199,7 +34371,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="11" t="e">
         <f>AVERAGEIF('Base SLA'!B3:B690,"&gt;0")</f>
@@ -34208,11 +34380,11 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B4" s="11">
         <f>AVERAGEIF('Base SLA'!C3:C690,"&gt;0")</f>
-        <v>63.272727272727273</v>
+        <v>68.728571428571428</v>
       </c>
     </row>
   </sheetData>
@@ -34224,26 +34396,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7271154-468d-4943-ad07-15f269a1f4f5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d241df49-fd27-41d8-ada8-b5e5272d8d25">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA29468F728387459F757BCD2E9F8EC0" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2a025e6ed7ca8ca0dee54093d0292095">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d241df49-fd27-41d8-ada8-b5e5272d8d25" xmlns:ns3="f7271154-468d-4943-ad07-15f269a1f4f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="07888a9383f211a4c31d7a2912379377" ns2:_="" ns3:_="">
     <xsd:import namespace="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
@@ -34492,26 +34644,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828E50A0-1F61-4B82-AF91-2402CEF44BFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7271154-468d-4943-ad07-15f269a1f4f5"/>
-    <ds:schemaRef ds:uri="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7271154-468d-4943-ad07-15f269a1f4f5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d241df49-fd27-41d8-ada8-b5e5272d8d25">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43F00D52-907D-4343-97A1-070EFC674BD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34528,4 +34681,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828E50A0-1F61-4B82-AF91-2402CEF44BFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7271154-468d-4943-ad07-15f269a1f4f5"/>
+    <ds:schemaRef ds:uri="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualizacao Planilha de Treinamentos dos Medicos 2
</commit_message>
<xml_diff>
--- a/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
+++ b/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD72227-44E1-49B6-AC46-72EDFC5D3DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AB42EB-0865-4F7E-A4FE-D8F1480B9ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F52E2CE3-F2BB-45A9-B9E9-D8B91065BEDA}"/>
   </bookViews>
@@ -2456,7 +2456,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z591"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -2569,7 +2568,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>103</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="62" t="s">
         <v>129</v>
       </c>
@@ -2685,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>198</v>
       </c>
@@ -2752,7 +2751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="62" t="s">
         <v>124</v>
       </c>
@@ -2815,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>105</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>50</v>
       </c>
@@ -2941,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>396</v>
       </c>
@@ -3008,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>290</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>218</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>176</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>78</v>
       </c>
@@ -3266,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>55</v>
       </c>
@@ -3329,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>38</v>
       </c>
@@ -3400,7 +3399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="62" t="s">
         <v>148</v>
       </c>
@@ -3461,7 +3460,7 @@
       <c r="X15" s="54"/>
       <c r="Y15" s="27"/>
     </row>
-    <row r="16" spans="1:25" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>400</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>107</v>
       </c>
@@ -3579,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>109</v>
       </c>
@@ -3642,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>426</v>
       </c>
@@ -3699,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:26" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>71</v>
       </c>
@@ -3761,7 +3760,7 @@
       </c>
       <c r="Z20"/>
     </row>
-    <row r="21" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>67</v>
       </c>
@@ -3826,7 +3825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>184</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>430</v>
       </c>
@@ -3940,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>167</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>169</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>172</v>
       </c>
@@ -4137,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>402</v>
       </c>
@@ -4190,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>404</v>
       </c>
@@ -4255,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>180</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="62" t="s">
         <v>137</v>
       </c>
@@ -4393,7 +4392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62" t="s">
         <v>147</v>
       </c>
@@ -4454,7 +4453,7 @@
       <c r="X31" s="54"/>
       <c r="Y31" s="27"/>
     </row>
-    <row r="32" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>267</v>
       </c>
@@ -4501,7 +4500,7 @@
       <c r="X32" s="54"/>
       <c r="Y32" s="27"/>
     </row>
-    <row r="33" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>80</v>
       </c>
@@ -4576,7 +4575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>312</v>
       </c>
@@ -4625,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>183</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>314</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>81</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="62" t="s">
         <v>125</v>
       </c>
@@ -4859,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>83</v>
       </c>
@@ -4922,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>223</v>
       </c>
@@ -4969,7 +4968,7 @@
       <c r="X40" s="54"/>
       <c r="Y40" s="27"/>
     </row>
-    <row r="41" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>53</v>
       </c>
@@ -5030,7 +5029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="62" t="s">
         <v>149</v>
       </c>
@@ -5091,7 +5090,7 @@
       <c r="X42" s="54"/>
       <c r="Y42" s="27"/>
     </row>
-    <row r="43" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="73" t="s">
         <v>164</v>
       </c>
@@ -5154,7 +5153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>248</v>
       </c>
@@ -5214,7 +5213,7 @@
       </c>
       <c r="Z44"/>
     </row>
-    <row r="45" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>61</v>
       </c>
@@ -5278,7 +5277,7 @@
       </c>
       <c r="Z45"/>
     </row>
-    <row r="46" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>57</v>
       </c>
@@ -5338,7 +5337,7 @@
       </c>
       <c r="Z46"/>
     </row>
-    <row r="47" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="62" t="s">
         <v>130</v>
       </c>
@@ -5392,7 +5391,7 @@
       </c>
       <c r="Z47"/>
     </row>
-    <row r="48" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>63</v>
       </c>
@@ -5454,7 +5453,7 @@
       </c>
       <c r="Z48"/>
     </row>
-    <row r="49" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>84</v>
       </c>
@@ -5532,7 +5531,7 @@
       </c>
       <c r="Z49"/>
     </row>
-    <row r="50" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="62" t="s">
         <v>126</v>
       </c>
@@ -5595,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>86</v>
       </c>
@@ -5668,7 +5667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
         <v>272</v>
       </c>
@@ -5715,7 +5714,7 @@
       <c r="X52" s="54"/>
       <c r="Y52" s="27"/>
     </row>
-    <row r="53" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>88</v>
       </c>
@@ -5778,7 +5777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="29" t="s">
         <v>32</v>
       </c>
@@ -5839,7 +5838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
         <v>89</v>
       </c>
@@ -5902,7 +5901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="78" t="s">
         <v>157</v>
       </c>
@@ -5963,7 +5962,7 @@
       <c r="X56" s="54"/>
       <c r="Y56" s="27"/>
     </row>
-    <row r="57" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="62" t="s">
         <v>127</v>
       </c>
@@ -6026,7 +6025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>173</v>
       </c>
@@ -6086,7 +6085,7 @@
       </c>
       <c r="Z58" s="19"/>
     </row>
-    <row r="59" spans="1:26" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="63" t="s">
         <v>258</v>
       </c>
@@ -6148,7 +6147,7 @@
       </c>
       <c r="Z59"/>
     </row>
-    <row r="60" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>220</v>
       </c>
@@ -6203,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="29" t="s">
         <v>22</v>
       </c>
@@ -6267,7 +6266,7 @@
       </c>
       <c r="Z61" s="19"/>
     </row>
-    <row r="62" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="62" t="s">
         <v>134</v>
       </c>
@@ -6330,7 +6329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
         <v>219</v>
       </c>
@@ -6397,7 +6396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15" t="s">
         <v>434</v>
       </c>
@@ -6455,7 +6454,7 @@
       </c>
       <c r="Z64" s="19"/>
     </row>
-    <row r="65" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
         <v>330</v>
       </c>
@@ -6504,7 +6503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="15" t="s">
         <v>174</v>
       </c>
@@ -6563,7 +6562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>90</v>
       </c>
@@ -6634,7 +6633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>91</v>
       </c>
@@ -6709,7 +6708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>437</v>
       </c>
@@ -6766,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15" t="s">
         <v>159</v>
       </c>
@@ -6829,7 +6828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>390</v>
       </c>
@@ -6884,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="62" t="s">
         <v>131</v>
       </c>
@@ -6935,7 +6934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
         <v>190</v>
       </c>
@@ -7012,7 +7011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="63" t="s">
         <v>259</v>
       </c>
@@ -7077,7 +7076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
         <v>111</v>
       </c>
@@ -7140,7 +7139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>73</v>
       </c>
@@ -7202,7 +7201,7 @@
       </c>
       <c r="Z76"/>
     </row>
-    <row r="77" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="62" t="s">
         <v>150</v>
       </c>
@@ -7263,7 +7262,7 @@
       <c r="X77" s="54"/>
       <c r="Y77" s="27"/>
     </row>
-    <row r="78" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>407</v>
       </c>
@@ -7328,7 +7327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="62" t="s">
         <v>139</v>
       </c>
@@ -7405,7 +7404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>256</v>
       </c>
@@ -7468,7 +7467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="s">
         <v>92</v>
       </c>
@@ -7546,7 +7545,7 @@
       </c>
       <c r="Z81"/>
     </row>
-    <row r="82" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="15" t="s">
         <v>221</v>
       </c>
@@ -7601,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="s">
         <v>160</v>
       </c>
@@ -7664,7 +7663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
         <v>161</v>
       </c>
@@ -7728,7 +7727,7 @@
       </c>
       <c r="Z84" s="19"/>
     </row>
-    <row r="85" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15" t="s">
         <v>201</v>
       </c>
@@ -7789,7 +7788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="15" t="s">
         <v>341</v>
       </c>
@@ -7838,7 +7837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
         <v>200</v>
       </c>
@@ -7899,7 +7898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="62" t="s">
         <v>151</v>
       </c>
@@ -7973,7 +7972,7 @@
       </c>
       <c r="Z88" s="19"/>
     </row>
-    <row r="89" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="79" t="s">
         <v>202</v>
       </c>
@@ -8032,7 +8031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="62" t="s">
         <v>140</v>
       </c>
@@ -8098,7 +8097,7 @@
       </c>
       <c r="Z90" s="19"/>
     </row>
-    <row r="91" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="63" t="s">
         <v>182</v>
       </c>
@@ -8160,7 +8159,7 @@
       </c>
       <c r="Z91" s="19"/>
     </row>
-    <row r="92" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="15" t="s">
         <v>93</v>
       </c>
@@ -8232,7 +8231,7 @@
       </c>
       <c r="Z92" s="19"/>
     </row>
-    <row r="93" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>347</v>
       </c>
@@ -8282,7 +8281,7 @@
       </c>
       <c r="Z93" s="19"/>
     </row>
-    <row r="94" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>95</v>
       </c>
@@ -8346,7 +8345,7 @@
       </c>
       <c r="Z94" s="19"/>
     </row>
-    <row r="95" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
         <v>170</v>
       </c>
@@ -8406,7 +8405,7 @@
       </c>
       <c r="Z95" s="19"/>
     </row>
-    <row r="96" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>113</v>
       </c>
@@ -8469,7 +8468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
         <v>163</v>
       </c>
@@ -8532,7 +8531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
         <v>445</v>
       </c>
@@ -8590,7 +8589,7 @@
       </c>
       <c r="Z98" s="19"/>
     </row>
-    <row r="99" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="15" t="s">
         <v>189</v>
       </c>
@@ -8652,7 +8651,7 @@
       </c>
       <c r="Z99"/>
     </row>
-    <row r="100" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
         <v>115</v>
       </c>
@@ -8715,7 +8714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="15" t="s">
         <v>175</v>
       </c>
@@ -8774,7 +8773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="15" t="s">
         <v>181</v>
       </c>
@@ -8837,7 +8836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="62" t="s">
         <v>152</v>
       </c>
@@ -8898,7 +8897,7 @@
       <c r="X103" s="54"/>
       <c r="Y103" s="93"/>
     </row>
-    <row r="104" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
         <v>197</v>
       </c>
@@ -8973,7 +8972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="62" t="s">
         <v>153</v>
       </c>
@@ -9034,7 +9033,7 @@
       <c r="X105" s="54"/>
       <c r="Y105" s="93"/>
     </row>
-    <row r="106" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="15" t="s">
         <v>185</v>
       </c>
@@ -9095,7 +9094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="15" t="s">
         <v>165</v>
       </c>
@@ -9158,7 +9157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="62" t="s">
         <v>141</v>
       </c>
@@ -9285,7 +9284,7 @@
       </c>
       <c r="Z109"/>
     </row>
-    <row r="110" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="15" t="s">
         <v>75</v>
       </c>
@@ -9337,7 +9336,7 @@
       </c>
       <c r="Z110"/>
     </row>
-    <row r="111" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
         <v>42</v>
       </c>
@@ -9399,7 +9398,7 @@
       </c>
       <c r="Z111"/>
     </row>
-    <row r="112" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="15" t="s">
         <v>410</v>
       </c>
@@ -9453,7 +9452,7 @@
       </c>
       <c r="Z112"/>
     </row>
-    <row r="113" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="15" t="s">
         <v>193</v>
       </c>
@@ -9530,7 +9529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="15" t="s">
         <v>412</v>
       </c>
@@ -9593,7 +9592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
         <v>284</v>
       </c>
@@ -9640,7 +9639,7 @@
       <c r="X115" s="54"/>
       <c r="Y115" s="93"/>
     </row>
-    <row r="116" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
         <v>192</v>
       </c>
@@ -9695,7 +9694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
         <v>119</v>
       </c>
@@ -9758,7 +9757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
         <v>216</v>
       </c>
@@ -9819,7 +9818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="15" t="s">
         <v>72</v>
       </c>
@@ -9945,7 +9944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="62" t="s">
         <v>142</v>
       </c>
@@ -10008,7 +10007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
         <v>171</v>
       </c>
@@ -10067,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="15" t="s">
         <v>361</v>
       </c>
@@ -10117,7 +10116,7 @@
       </c>
       <c r="Z123"/>
     </row>
-    <row r="124" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="15" t="s">
         <v>76</v>
       </c>
@@ -10181,7 +10180,7 @@
       </c>
       <c r="Z124"/>
     </row>
-    <row r="125" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="15" t="s">
         <v>415</v>
       </c>
@@ -10234,7 +10233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="15" t="s">
         <v>178</v>
       </c>
@@ -10289,7 +10288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="15" t="s">
         <v>450</v>
       </c>
@@ -10347,7 +10346,7 @@
       </c>
       <c r="Z127"/>
     </row>
-    <row r="128" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="15" t="s">
         <v>98</v>
       </c>
@@ -10424,7 +10423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="15" t="s">
         <v>166</v>
       </c>
@@ -10487,7 +10486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="62" t="s">
         <v>155</v>
       </c>
@@ -10550,7 +10549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="15" t="s">
         <v>215</v>
       </c>
@@ -10611,7 +10610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="15" t="s">
         <v>417</v>
       </c>
@@ -10664,7 +10663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="15" t="s">
         <v>49</v>
       </c>
@@ -10726,7 +10725,7 @@
       </c>
       <c r="Z133"/>
     </row>
-    <row r="134" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="62" t="s">
         <v>132</v>
       </c>
@@ -10790,7 +10789,7 @@
       </c>
       <c r="Z134"/>
     </row>
-    <row r="135" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="15" t="s">
         <v>453</v>
       </c>
@@ -10843,7 +10842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="62" t="s">
         <v>143</v>
       </c>
@@ -10916,7 +10915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="63" t="s">
         <v>214</v>
       </c>
@@ -10977,7 +10976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="15" t="s">
         <v>74</v>
       </c>
@@ -11040,7 +11039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="15" t="s">
         <v>99</v>
       </c>
@@ -11114,7 +11113,7 @@
       </c>
       <c r="Z139" s="19"/>
     </row>
-    <row r="140" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="15" t="s">
         <v>177</v>
       </c>
@@ -11177,7 +11176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="15" t="s">
         <v>47</v>
       </c>
@@ -11240,7 +11239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="15" t="s">
         <v>419</v>
       </c>
@@ -11318,7 +11317,7 @@
       </c>
       <c r="Z142" s="19"/>
     </row>
-    <row r="143" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="15" t="s">
         <v>121</v>
       </c>
@@ -11381,7 +11380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="15" t="s">
         <v>54</v>
       </c>
@@ -11442,7 +11441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="15" t="s">
         <v>370</v>
       </c>
@@ -11492,7 +11491,7 @@
       </c>
       <c r="Z145" s="19"/>
     </row>
-    <row r="146" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="19" t="s">
         <v>77</v>
       </c>
@@ -11544,7 +11543,7 @@
       </c>
       <c r="Z146"/>
     </row>
-    <row r="147" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="15" t="s">
         <v>194</v>
       </c>
@@ -11605,7 +11604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="15" t="s">
         <v>100</v>
       </c>
@@ -11669,7 +11668,7 @@
       </c>
       <c r="Z148"/>
     </row>
-    <row r="149" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="62" t="s">
         <v>144</v>
       </c>
@@ -11732,7 +11731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="15" t="s">
         <v>101</v>
       </c>
@@ -11807,7 +11806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="15" t="s">
         <v>69</v>
       </c>
@@ -11882,7 +11881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="15" t="s">
         <v>217</v>
       </c>
@@ -12004,7 +12003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="15" t="s">
         <v>44</v>
       </c>
@@ -12065,7 +12064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="15" t="s">
         <v>196</v>
       </c>
@@ -12127,7 +12126,7 @@
       </c>
       <c r="Z155" s="19"/>
     </row>
-    <row r="156" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="62" t="s">
         <v>154</v>
       </c>
@@ -12189,7 +12188,7 @@
       <c r="Y156" s="93"/>
       <c r="Z156" s="19"/>
     </row>
-    <row r="157" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="15" t="s">
         <v>222</v>
       </c>
@@ -12264,7 +12263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="62" t="s">
         <v>145</v>
       </c>
@@ -12326,7 +12325,7 @@
       </c>
       <c r="Z158" s="19"/>
     </row>
-    <row r="159" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="15" t="s">
         <v>381</v>
       </c>
@@ -12376,7 +12375,7 @@
       </c>
       <c r="Z159" s="19"/>
     </row>
-    <row r="160" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="15" t="s">
         <v>186</v>
       </c>
@@ -12438,7 +12437,7 @@
       </c>
       <c r="Z160" s="19"/>
     </row>
-    <row r="161" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="62" t="s">
         <v>146</v>
       </c>
@@ -12501,7 +12500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="19" t="s">
         <v>191</v>
       </c>
@@ -12562,7 +12561,7 @@
       <c r="X162" s="54"/>
       <c r="Y162" s="93"/>
     </row>
-    <row r="163" spans="1:26" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="15" t="s">
         <v>187</v>
       </c>
@@ -12624,7 +12623,7 @@
       </c>
       <c r="Z163" s="19"/>
     </row>
-    <row r="164" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="15" t="s">
         <v>64</v>
       </c>
@@ -12688,7 +12687,7 @@
       </c>
       <c r="Z164"/>
     </row>
-    <row r="165" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="15" t="s">
         <v>199</v>
       </c>
@@ -12749,7 +12748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:26" s="19" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="15" t="s">
         <v>188</v>
       </c>
@@ -24712,11 +24711,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Z166" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
-    <filterColumn colId="18">
-      <filters>
-        <filter val="NÃO COMPARECEU"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z166">
       <sortCondition ref="A1:A166"/>
     </sortState>
@@ -34306,15 +34300,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7271154-468d-4943-ad07-15f269a1f4f5" xsi:nil="true"/>
@@ -34323,6 +34308,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34575,20 +34569,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828E50A0-1F61-4B82-AF91-2402CEF44BFC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f7271154-468d-4943-ad07-15f269a1f4f5"/>
     <ds:schemaRef ds:uri="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Atualizacao Planilha de Treinamentos dos Medicos 3
</commit_message>
<xml_diff>
--- a/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
+++ b/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AB42EB-0865-4F7E-A4FE-D8F1480B9ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1E4DE6-5B1E-45B1-ADE9-308656F7D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F52E2CE3-F2BB-45A9-B9E9-D8B91065BEDA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="463">
   <si>
     <t>Nome do Médico</t>
   </si>
@@ -1913,7 +1913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2137,6 +2137,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2458,9 +2487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
   <dimension ref="A1:Z591"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W153" sqref="W153"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A166" sqref="A166:XFD166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2680,7 +2709,7 @@
         <v>30</v>
       </c>
       <c r="X3" s="54"/>
-      <c r="Y3" s="27">
+      <c r="Y3" s="40">
         <v>0</v>
       </c>
     </row>
@@ -3050,7 +3079,9 @@
       <c r="T9" s="67"/>
       <c r="U9" s="67"/>
       <c r="V9" s="67"/>
-      <c r="W9" s="15"/>
+      <c r="W9" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X9" s="54"/>
       <c r="Y9" s="40">
         <v>0</v>
@@ -3255,8 +3286,8 @@
       <c r="V12" s="52" t="s">
         <v>295</v>
       </c>
-      <c r="W12" s="15" t="s">
-        <v>296</v>
+      <c r="W12" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X12" s="40" t="s">
         <v>31</v>
@@ -3391,7 +3422,9 @@
       </c>
       <c r="U14" s="37"/>
       <c r="V14" s="37"/>
-      <c r="W14" s="15"/>
+      <c r="W14" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X14" s="40" t="s">
         <v>31</v>
       </c>
@@ -3456,9 +3489,13 @@
       <c r="T15" s="48"/>
       <c r="U15" s="48"/>
       <c r="V15" s="48"/>
-      <c r="W15" s="15"/>
+      <c r="W15" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X15" s="54"/>
-      <c r="Y15" s="27"/>
+      <c r="Y15" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
@@ -3817,7 +3854,9 @@
       </c>
       <c r="U21" s="37"/>
       <c r="V21" s="37"/>
-      <c r="W21" s="15"/>
+      <c r="W21" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X21" s="40" t="s">
         <v>31</v>
       </c>
@@ -3880,7 +3919,9 @@
       <c r="T22" s="67"/>
       <c r="U22" s="67"/>
       <c r="V22" s="67"/>
-      <c r="W22" s="15"/>
+      <c r="W22" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X22" s="54"/>
       <c r="Y22" s="40">
         <v>0</v>
@@ -3996,7 +4037,9 @@
       <c r="T24" s="67"/>
       <c r="U24" s="67"/>
       <c r="V24" s="67"/>
-      <c r="W24" s="15"/>
+      <c r="W24" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X24" s="54"/>
       <c r="Y24" s="40">
         <v>0</v>
@@ -4130,7 +4173,9 @@
       <c r="T26" s="67"/>
       <c r="U26" s="67"/>
       <c r="V26" s="67"/>
-      <c r="W26" s="15"/>
+      <c r="W26" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X26" s="54"/>
       <c r="Y26" s="40">
         <v>0</v>
@@ -4309,7 +4354,9 @@
       <c r="T29" s="67"/>
       <c r="U29" s="67"/>
       <c r="V29" s="67"/>
-      <c r="W29" s="15"/>
+      <c r="W29" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X29" s="54"/>
       <c r="Y29" s="40">
         <v>0</v>
@@ -4449,9 +4496,13 @@
       <c r="T31" s="48"/>
       <c r="U31" s="48"/>
       <c r="V31" s="48"/>
-      <c r="W31" s="15"/>
+      <c r="W31" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X31" s="54"/>
-      <c r="Y31" s="27"/>
+      <c r="Y31" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
@@ -4496,9 +4547,13 @@
       <c r="T32" s="67"/>
       <c r="U32" s="67"/>
       <c r="V32" s="67"/>
-      <c r="W32" s="15"/>
+      <c r="W32" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X32" s="54"/>
-      <c r="Y32" s="27"/>
+      <c r="Y32" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
@@ -4567,7 +4622,9 @@
       <c r="V33" s="52" t="s">
         <v>255</v>
       </c>
-      <c r="W33" s="15"/>
+      <c r="W33" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X33" s="40" t="s">
         <v>31</v>
       </c>
@@ -4618,7 +4675,9 @@
       <c r="T34" s="67"/>
       <c r="U34" s="67"/>
       <c r="V34" s="67"/>
-      <c r="W34" s="15"/>
+      <c r="W34" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X34" s="54"/>
       <c r="Y34" s="40">
         <v>0</v>
@@ -4728,7 +4787,9 @@
       <c r="T36" s="67"/>
       <c r="U36" s="67"/>
       <c r="V36" s="67"/>
-      <c r="W36" s="15"/>
+      <c r="W36" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X36" s="54"/>
       <c r="Y36" s="40">
         <v>0</v>
@@ -4799,7 +4860,9 @@
         <v>317</v>
       </c>
       <c r="V37" s="49"/>
-      <c r="W37" s="15"/>
+      <c r="W37" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X37" s="40" t="s">
         <v>31</v>
       </c>
@@ -4854,7 +4917,7 @@
         <v>30</v>
       </c>
       <c r="X38" s="54"/>
-      <c r="Y38" s="27">
+      <c r="Y38" s="40">
         <v>0</v>
       </c>
     </row>
@@ -4915,7 +4978,9 @@
       <c r="T39" s="48"/>
       <c r="U39" s="48"/>
       <c r="V39" s="48"/>
-      <c r="W39" s="15"/>
+      <c r="W39" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X39" s="54"/>
       <c r="Y39" s="40">
         <v>0</v>
@@ -4964,9 +5029,13 @@
       <c r="T40" s="67"/>
       <c r="U40" s="67"/>
       <c r="V40" s="67"/>
-      <c r="W40" s="15"/>
+      <c r="W40" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X40" s="54"/>
-      <c r="Y40" s="27"/>
+      <c r="Y40" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
@@ -5086,9 +5155,13 @@
       <c r="T42" s="48"/>
       <c r="U42" s="48"/>
       <c r="V42" s="48"/>
-      <c r="W42" s="15"/>
+      <c r="W42" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X42" s="54"/>
-      <c r="Y42" s="27"/>
+      <c r="Y42" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="73" t="s">
@@ -5332,7 +5405,7 @@
         <v>30</v>
       </c>
       <c r="X46" s="54"/>
-      <c r="Y46" s="27">
+      <c r="Y46" s="40">
         <v>0</v>
       </c>
       <c r="Z46"/>
@@ -5386,7 +5459,7 @@
         <v>30</v>
       </c>
       <c r="X47" s="54"/>
-      <c r="Y47" s="27">
+      <c r="Y47" s="40">
         <v>0</v>
       </c>
       <c r="Z47"/>
@@ -5520,8 +5593,8 @@
       <c r="V49" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="W49" s="15" t="s">
-        <v>296</v>
+      <c r="W49" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X49" s="40" t="s">
         <v>31</v>
@@ -5659,7 +5732,9 @@
         <v>324</v>
       </c>
       <c r="V51" s="49"/>
-      <c r="W51" s="15"/>
+      <c r="W51" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X51" s="40" t="s">
         <v>31</v>
       </c>
@@ -5710,9 +5785,13 @@
       <c r="T52" s="67"/>
       <c r="U52" s="67"/>
       <c r="V52" s="67"/>
-      <c r="W52" s="15"/>
+      <c r="W52" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X52" s="54"/>
-      <c r="Y52" s="27"/>
+      <c r="Y52" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
@@ -5771,7 +5850,9 @@
       <c r="T53" s="48"/>
       <c r="U53" s="48"/>
       <c r="V53" s="48"/>
-      <c r="W53" s="15"/>
+      <c r="W53" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X53" s="54"/>
       <c r="Y53" s="40">
         <v>0</v>
@@ -5895,7 +5976,9 @@
       <c r="T55" s="48"/>
       <c r="U55" s="48"/>
       <c r="V55" s="48"/>
-      <c r="W55" s="15"/>
+      <c r="W55" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X55" s="54"/>
       <c r="Y55" s="40">
         <v>0</v>
@@ -5958,9 +6041,13 @@
       <c r="T56" s="48"/>
       <c r="U56" s="48"/>
       <c r="V56" s="48"/>
-      <c r="W56" s="15"/>
+      <c r="W56" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X56" s="54"/>
-      <c r="Y56" s="27"/>
+      <c r="Y56" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="62" t="s">
@@ -6078,74 +6165,77 @@
       <c r="T58" s="67"/>
       <c r="U58" s="67"/>
       <c r="V58" s="67"/>
-      <c r="W58" s="15"/>
+      <c r="W58" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X58" s="54"/>
       <c r="Y58" s="40">
         <v>0</v>
       </c>
       <c r="Z58" s="19"/>
     </row>
-    <row r="59" spans="1:26" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="63" t="s">
+    <row r="59" spans="1:26" s="107" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="95" t="s">
         <v>258</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="E59" s="20" t="s">
+      <c r="E59" s="97" t="s">
         <v>329</v>
       </c>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H59" s="31">
+      <c r="F59" s="97"/>
+      <c r="G59" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="98">
         <v>45267</v>
       </c>
-      <c r="I59" s="85" t="s">
+      <c r="I59" s="99" t="s">
         <v>303</v>
       </c>
-      <c r="J59" s="31" t="s">
+      <c r="J59" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="K59" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="L59" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="M59" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="N59" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="O59" s="35" t="s">
+      <c r="K59" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="L59" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="M59" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="N59" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="O59" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="P59" s="31" t="s">
+      <c r="P59" s="98" t="s">
         <v>225</v>
       </c>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="51"/>
-      <c r="S59" s="48" t="s">
+      <c r="Q59" s="96"/>
+      <c r="R59" s="101"/>
+      <c r="S59" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="T59" s="67"/>
-      <c r="U59" s="67"/>
-      <c r="V59" s="67"/>
-      <c r="W59" s="15"/>
-      <c r="X59" s="54"/>
-      <c r="Y59" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z59"/>
+      <c r="T59" s="103"/>
+      <c r="U59" s="103"/>
+      <c r="V59" s="103"/>
+      <c r="W59" s="104" t="s">
+        <v>30</v>
+      </c>
+      <c r="X59" s="105"/>
+      <c r="Y59" s="106">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
@@ -6198,7 +6288,7 @@
         <v>30</v>
       </c>
       <c r="X60" s="54"/>
-      <c r="Y60" s="27">
+      <c r="Y60" s="40">
         <v>0</v>
       </c>
     </row>
@@ -6497,7 +6587,9 @@
       <c r="T65" s="58"/>
       <c r="U65" s="67"/>
       <c r="V65" s="67"/>
-      <c r="W65" s="15"/>
+      <c r="W65" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X65" s="54"/>
       <c r="Y65" s="40">
         <v>0</v>
@@ -6556,7 +6648,9 @@
       <c r="T66" s="67"/>
       <c r="U66" s="67"/>
       <c r="V66" s="67"/>
-      <c r="W66" s="15"/>
+      <c r="W66" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X66" s="54"/>
       <c r="Y66" s="40">
         <v>0</v>
@@ -6625,7 +6719,9 @@
       </c>
       <c r="U67" s="48"/>
       <c r="V67" s="48"/>
-      <c r="W67" s="15"/>
+      <c r="W67" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X67" s="40" t="s">
         <v>31</v>
       </c>
@@ -6698,8 +6794,8 @@
       <c r="V68" s="52" t="s">
         <v>337</v>
       </c>
-      <c r="W68" s="15" t="s">
-        <v>296</v>
+      <c r="W68" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X68" s="40" t="s">
         <v>31</v>
@@ -6879,7 +6975,7 @@
         <v>30</v>
       </c>
       <c r="X71" s="54"/>
-      <c r="Y71" s="27">
+      <c r="Y71" s="40">
         <v>0</v>
       </c>
     </row>
@@ -6930,7 +7026,7 @@
         <v>30</v>
       </c>
       <c r="X72" s="54"/>
-      <c r="Y72" s="27">
+      <c r="Y72" s="40">
         <v>0</v>
       </c>
     </row>
@@ -7001,8 +7097,8 @@
       <c r="V73" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="W73" s="15" t="s">
-        <v>296</v>
+      <c r="W73" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X73" s="40" t="s">
         <v>31</v>
@@ -7258,9 +7354,13 @@
       <c r="T77" s="48"/>
       <c r="U77" s="48"/>
       <c r="V77" s="48"/>
-      <c r="W77" s="15"/>
+      <c r="W77" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X77" s="54"/>
-      <c r="Y77" s="27"/>
+      <c r="Y77" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
@@ -7534,8 +7634,8 @@
       <c r="V81" s="52" t="s">
         <v>253</v>
       </c>
-      <c r="W81" s="15" t="s">
-        <v>296</v>
+      <c r="W81" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X81" s="40" t="s">
         <v>31</v>
@@ -7596,7 +7696,7 @@
         <v>30</v>
       </c>
       <c r="X82" s="54"/>
-      <c r="Y82" s="93">
+      <c r="Y82" s="40">
         <v>0</v>
       </c>
     </row>
@@ -7831,9 +7931,11 @@
       <c r="T86" s="67"/>
       <c r="U86" s="67"/>
       <c r="V86" s="67"/>
-      <c r="W86" s="15"/>
+      <c r="W86" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X86" s="54"/>
-      <c r="Y86" s="39">
+      <c r="Y86" s="40">
         <v>0</v>
       </c>
     </row>
@@ -7892,9 +7994,11 @@
       <c r="T87" s="67"/>
       <c r="U87" s="67"/>
       <c r="V87" s="67"/>
-      <c r="W87" s="15"/>
+      <c r="W87" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X87" s="54"/>
-      <c r="Y87" s="39">
+      <c r="Y87" s="40">
         <v>0</v>
       </c>
     </row>
@@ -7963,7 +8067,9 @@
         <v>250</v>
       </c>
       <c r="V88" s="49"/>
-      <c r="W88" s="15"/>
+      <c r="W88" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X88" s="40" t="s">
         <v>31</v>
       </c>
@@ -8027,7 +8133,7 @@
         <v>30</v>
       </c>
       <c r="X89" s="77"/>
-      <c r="Y89" s="39">
+      <c r="Y89" s="40">
         <v>0</v>
       </c>
     </row>
@@ -8092,7 +8198,7 @@
         <v>30</v>
       </c>
       <c r="X90" s="54"/>
-      <c r="Y90" s="39">
+      <c r="Y90" s="40">
         <v>0</v>
       </c>
       <c r="Z90" s="19"/>
@@ -8152,9 +8258,11 @@
       <c r="T91" s="67"/>
       <c r="U91" s="67"/>
       <c r="V91" s="67"/>
-      <c r="W91" s="15"/>
+      <c r="W91" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X91" s="54"/>
-      <c r="Y91" s="39">
+      <c r="Y91" s="40">
         <v>0</v>
       </c>
       <c r="Z91" s="19"/>
@@ -8222,7 +8330,9 @@
       </c>
       <c r="U92" s="48"/>
       <c r="V92" s="48"/>
-      <c r="W92" s="15"/>
+      <c r="W92" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X92" s="40" t="s">
         <v>31</v>
       </c>
@@ -8274,9 +8384,11 @@
       <c r="T93" s="67"/>
       <c r="U93" s="67"/>
       <c r="V93" s="67"/>
-      <c r="W93" s="15"/>
+      <c r="W93" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X93" s="54"/>
-      <c r="Y93" s="39">
+      <c r="Y93" s="40">
         <v>0</v>
       </c>
       <c r="Z93" s="19"/>
@@ -8338,9 +8450,11 @@
       <c r="T94" s="48"/>
       <c r="U94" s="48"/>
       <c r="V94" s="48"/>
-      <c r="W94" s="15"/>
+      <c r="W94" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X94" s="54"/>
-      <c r="Y94" s="39">
+      <c r="Y94" s="40">
         <v>0</v>
       </c>
       <c r="Z94" s="19"/>
@@ -8398,9 +8512,11 @@
       <c r="T95" s="67"/>
       <c r="U95" s="67"/>
       <c r="V95" s="67"/>
-      <c r="W95" s="15"/>
+      <c r="W95" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X95" s="54"/>
-      <c r="Y95" s="39">
+      <c r="Y95" s="40">
         <v>0</v>
       </c>
       <c r="Z95" s="19"/>
@@ -8584,7 +8700,7 @@
         <v>30</v>
       </c>
       <c r="X98" s="54"/>
-      <c r="Y98" s="39">
+      <c r="Y98" s="40">
         <v>0</v>
       </c>
       <c r="Z98" s="19"/>
@@ -8767,9 +8883,11 @@
       <c r="T101" s="67"/>
       <c r="U101" s="67"/>
       <c r="V101" s="67"/>
-      <c r="W101" s="15"/>
+      <c r="W101" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X101" s="54"/>
-      <c r="Y101" s="39">
+      <c r="Y101" s="40">
         <v>0</v>
       </c>
     </row>
@@ -8893,9 +9011,13 @@
       <c r="T103" s="48"/>
       <c r="U103" s="48"/>
       <c r="V103" s="48"/>
-      <c r="W103" s="15"/>
+      <c r="W103" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X103" s="54"/>
-      <c r="Y103" s="93"/>
+      <c r="Y103" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
@@ -8962,8 +9084,8 @@
       <c r="V104" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="W104" s="15" t="s">
-        <v>296</v>
+      <c r="W104" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X104" s="40" t="s">
         <v>31</v>
@@ -9029,9 +9151,13 @@
       <c r="T105" s="48"/>
       <c r="U105" s="48"/>
       <c r="V105" s="48"/>
-      <c r="W105" s="15"/>
+      <c r="W105" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X105" s="54"/>
-      <c r="Y105" s="93"/>
+      <c r="Y105" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="15" t="s">
@@ -9088,9 +9214,11 @@
       <c r="T106" s="67"/>
       <c r="U106" s="67"/>
       <c r="V106" s="67"/>
-      <c r="W106" s="15"/>
+      <c r="W106" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X106" s="54"/>
-      <c r="Y106" s="39">
+      <c r="Y106" s="40">
         <v>0</v>
       </c>
     </row>
@@ -9279,7 +9407,7 @@
         <v>30</v>
       </c>
       <c r="X109" s="54"/>
-      <c r="Y109" s="93">
+      <c r="Y109" s="40">
         <v>0</v>
       </c>
       <c r="Z109"/>
@@ -9331,7 +9459,7 @@
         <v>30</v>
       </c>
       <c r="X110" s="54"/>
-      <c r="Y110" s="93">
+      <c r="Y110" s="40">
         <v>0</v>
       </c>
       <c r="Z110"/>
@@ -9447,7 +9575,7 @@
         <v>30</v>
       </c>
       <c r="X112" s="54"/>
-      <c r="Y112" s="39">
+      <c r="Y112" s="40">
         <v>0</v>
       </c>
       <c r="Z112"/>
@@ -9519,8 +9647,8 @@
       <c r="V113" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="W113" s="15" t="s">
-        <v>296</v>
+      <c r="W113" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X113" s="40" t="s">
         <v>31</v>
@@ -9588,7 +9716,7 @@
         <v>30</v>
       </c>
       <c r="X114" s="54"/>
-      <c r="Y114" s="39">
+      <c r="Y114" s="40">
         <v>0</v>
       </c>
     </row>
@@ -9635,9 +9763,13 @@
       <c r="T115" s="67"/>
       <c r="U115" s="67"/>
       <c r="V115" s="67"/>
-      <c r="W115" s="15"/>
+      <c r="W115" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X115" s="54"/>
-      <c r="Y115" s="93"/>
+      <c r="Y115" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
@@ -9689,7 +9821,9 @@
       <c r="W116" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="X116" s="54"/>
+      <c r="X116" s="40" t="s">
+        <v>31</v>
+      </c>
       <c r="Y116" s="39">
         <v>1</v>
       </c>
@@ -9812,9 +9946,11 @@
       <c r="T118" s="58"/>
       <c r="U118" s="67"/>
       <c r="V118" s="67"/>
-      <c r="W118" s="15"/>
+      <c r="W118" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X118" s="54"/>
-      <c r="Y118" s="39">
+      <c r="Y118" s="40">
         <v>0</v>
       </c>
     </row>
@@ -9940,7 +10076,7 @@
         <v>30</v>
       </c>
       <c r="X120" s="54"/>
-      <c r="Y120" s="39">
+      <c r="Y120" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10003,7 +10139,7 @@
         <v>30</v>
       </c>
       <c r="X121" s="54"/>
-      <c r="Y121" s="39">
+      <c r="Y121" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10060,9 +10196,11 @@
       <c r="T122" s="58"/>
       <c r="U122" s="67"/>
       <c r="V122" s="67"/>
-      <c r="W122" s="15"/>
+      <c r="W122" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X122" s="54"/>
-      <c r="Y122" s="39">
+      <c r="Y122" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10109,9 +10247,11 @@
       <c r="T123" s="67"/>
       <c r="U123" s="67"/>
       <c r="V123" s="67"/>
-      <c r="W123" s="15"/>
+      <c r="W123" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X123" s="54"/>
-      <c r="Y123" s="39">
+      <c r="Y123" s="40">
         <v>0</v>
       </c>
       <c r="Z123"/>
@@ -10229,7 +10369,7 @@
         <v>30</v>
       </c>
       <c r="X125" s="54"/>
-      <c r="Y125" s="39">
+      <c r="Y125" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10284,7 +10424,7 @@
         <v>30</v>
       </c>
       <c r="X126" s="54"/>
-      <c r="Y126" s="39">
+      <c r="Y126" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10341,7 +10481,7 @@
         <v>30</v>
       </c>
       <c r="X127" s="54"/>
-      <c r="Y127" s="39">
+      <c r="Y127" s="40">
         <v>0</v>
       </c>
       <c r="Z127"/>
@@ -10604,9 +10744,11 @@
       <c r="T131" s="67"/>
       <c r="U131" s="67"/>
       <c r="V131" s="67"/>
-      <c r="W131" s="15"/>
+      <c r="W131" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X131" s="54"/>
-      <c r="Y131" s="39">
+      <c r="Y131" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10659,7 +10801,7 @@
         <v>30</v>
       </c>
       <c r="X132" s="54"/>
-      <c r="Y132" s="39">
+      <c r="Y132" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10838,7 +10980,7 @@
         <v>30</v>
       </c>
       <c r="X135" s="54"/>
-      <c r="Y135" s="39">
+      <c r="Y135" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10970,9 +11112,11 @@
       <c r="T137" s="67"/>
       <c r="U137" s="67"/>
       <c r="V137" s="67"/>
-      <c r="W137" s="15"/>
+      <c r="W137" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X137" s="54"/>
-      <c r="Y137" s="39">
+      <c r="Y137" s="40">
         <v>0</v>
       </c>
     </row>
@@ -11104,7 +11248,9 @@
         <v>324</v>
       </c>
       <c r="V139" s="46"/>
-      <c r="W139" s="15"/>
+      <c r="W139" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X139" s="40" t="s">
         <v>31</v>
       </c>
@@ -11484,9 +11630,11 @@
       <c r="T145" s="67"/>
       <c r="U145" s="67"/>
       <c r="V145" s="67"/>
-      <c r="W145" s="15"/>
+      <c r="W145" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X145" s="15"/>
-      <c r="Y145" s="39">
+      <c r="Y145" s="40">
         <v>0</v>
       </c>
       <c r="Z145" s="19"/>
@@ -11538,7 +11686,7 @@
         <v>30</v>
       </c>
       <c r="X146" s="15"/>
-      <c r="Y146" s="93">
+      <c r="Y146" s="40">
         <v>0</v>
       </c>
       <c r="Z146"/>
@@ -11598,9 +11746,11 @@
       <c r="T147" s="67"/>
       <c r="U147" s="67"/>
       <c r="V147" s="67"/>
-      <c r="W147" s="15"/>
+      <c r="W147" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X147" s="15"/>
-      <c r="Y147" s="39">
+      <c r="Y147" s="40">
         <v>0</v>
       </c>
     </row>
@@ -11661,9 +11811,11 @@
       <c r="T148" s="48"/>
       <c r="U148" s="48"/>
       <c r="V148" s="48"/>
-      <c r="W148" s="15"/>
+      <c r="W148" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X148" s="54"/>
-      <c r="Y148" s="39">
+      <c r="Y148" s="40">
         <v>0</v>
       </c>
       <c r="Z148"/>
@@ -11727,7 +11879,7 @@
         <v>30</v>
       </c>
       <c r="X149" s="54"/>
-      <c r="Y149" s="39">
+      <c r="Y149" s="40">
         <v>0</v>
       </c>
     </row>
@@ -11796,8 +11948,8 @@
       <c r="V150" s="52" t="s">
         <v>253</v>
       </c>
-      <c r="W150" s="15" t="s">
-        <v>296</v>
+      <c r="W150" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="X150" s="40" t="s">
         <v>31</v>
@@ -11999,7 +12151,7 @@
         <v>30</v>
       </c>
       <c r="X153" s="54"/>
-      <c r="Y153" s="39">
+      <c r="Y153" s="40">
         <v>0</v>
       </c>
     </row>
@@ -12119,9 +12271,11 @@
       <c r="T155" s="67"/>
       <c r="U155" s="67"/>
       <c r="V155" s="67"/>
-      <c r="W155" s="15"/>
+      <c r="W155" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X155" s="54"/>
-      <c r="Y155" s="39">
+      <c r="Y155" s="40">
         <v>0</v>
       </c>
       <c r="Z155" s="19"/>
@@ -12183,9 +12337,13 @@
       <c r="T156" s="48"/>
       <c r="U156" s="48"/>
       <c r="V156" s="48"/>
-      <c r="W156" s="15"/>
+      <c r="W156" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X156" s="54"/>
-      <c r="Y156" s="93"/>
+      <c r="Y156" s="40">
+        <v>0</v>
+      </c>
       <c r="Z156" s="19"/>
     </row>
     <row r="157" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12320,7 +12478,7 @@
         <v>30</v>
       </c>
       <c r="X158" s="54"/>
-      <c r="Y158" s="39">
+      <c r="Y158" s="40">
         <v>0</v>
       </c>
       <c r="Z158" s="19"/>
@@ -12368,9 +12526,11 @@
       <c r="T159" s="67"/>
       <c r="U159" s="67"/>
       <c r="V159" s="67"/>
-      <c r="W159" s="15"/>
+      <c r="W159" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X159" s="54"/>
-      <c r="Y159" s="39">
+      <c r="Y159" s="40">
         <v>0</v>
       </c>
       <c r="Z159" s="19"/>
@@ -12430,9 +12590,11 @@
       <c r="T160" s="58"/>
       <c r="U160" s="67"/>
       <c r="V160" s="67"/>
-      <c r="W160" s="15"/>
+      <c r="W160" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X160" s="54"/>
-      <c r="Y160" s="39">
+      <c r="Y160" s="40">
         <v>0</v>
       </c>
       <c r="Z160" s="19"/>
@@ -12496,7 +12658,7 @@
         <v>30</v>
       </c>
       <c r="X161" s="54"/>
-      <c r="Y161" s="39">
+      <c r="Y161" s="40">
         <v>0</v>
       </c>
     </row>
@@ -12557,9 +12719,13 @@
       <c r="T162" s="67"/>
       <c r="U162" s="67"/>
       <c r="V162" s="67"/>
-      <c r="W162" s="15"/>
+      <c r="W162" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X162" s="54"/>
-      <c r="Y162" s="93"/>
+      <c r="Y162" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="163" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="15" t="s">
@@ -12616,9 +12782,11 @@
       <c r="T163" s="67"/>
       <c r="U163" s="67"/>
       <c r="V163" s="67"/>
-      <c r="W163" s="15"/>
+      <c r="W163" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X163" s="54"/>
-      <c r="Y163" s="39">
+      <c r="Y163" s="40">
         <v>0</v>
       </c>
       <c r="Z163" s="19"/>
@@ -12742,13 +12910,15 @@
       <c r="T165" s="67"/>
       <c r="U165" s="67"/>
       <c r="V165" s="67"/>
-      <c r="W165" s="15"/>
+      <c r="W165" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X165" s="54"/>
-      <c r="Y165" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:26" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y165" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:26" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="15" t="s">
         <v>188</v>
       </c>
@@ -12803,9 +12973,11 @@
       <c r="T166" s="67"/>
       <c r="U166" s="67"/>
       <c r="V166" s="67"/>
-      <c r="W166" s="15"/>
+      <c r="W166" s="39" t="s">
+        <v>30</v>
+      </c>
       <c r="X166" s="54"/>
-      <c r="Y166" s="39">
+      <c r="Y166" s="40">
         <v>0</v>
       </c>
     </row>
@@ -34300,6 +34472,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7271154-468d-4943-ad07-15f269a1f4f5" xsi:nil="true"/>
@@ -34308,15 +34489,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34569,20 +34741,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828E50A0-1F61-4B82-AF91-2402CEF44BFC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f7271154-468d-4943-ad07-15f269a1f4f5"/>
     <ds:schemaRef ds:uri="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Exclusao Pagina Realizado - Reestruturacao dos Graficos
</commit_message>
<xml_diff>
--- a/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
+++ b/prj_imunomediados _controle_onboarding_21_02_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keller\Documents\Projetos\Cursos\Python\Dashboard_Area_Logada\Area_Logada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4F0D3D-32BF-4C20-8817-47B23038EA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470597B-3C81-4627-96B0-8915E20EA4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F52E2CE3-F2BB-45A9-B9E9-D8B91065BEDA}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="SLAs" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados_Onboarding!$A$1:$Z$241</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados_Onboarding!$A$1:$Y$241</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4495" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4477" uniqueCount="986">
   <si>
     <t>Nome do Médico</t>
   </si>
@@ -4944,9 +4944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C803E3-8D15-4C2F-A516-8FD35CD8D5C2}">
   <dimension ref="A1:Z354"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S133" sqref="S133"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P243" sqref="P243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5706,8 +5706,8 @@
         <v>23</v>
       </c>
       <c r="O11" s="170"/>
-      <c r="P11" s="44" t="s">
-        <v>197</v>
+      <c r="P11" s="51">
+        <v>45292</v>
       </c>
       <c r="Q11" s="137"/>
       <c r="R11" s="44" t="s">
@@ -7006,8 +7006,8 @@
       <c r="O29" s="247" t="s">
         <v>461</v>
       </c>
-      <c r="P29" s="44" t="s">
-        <v>197</v>
+      <c r="P29" s="51">
+        <v>45292</v>
       </c>
       <c r="Q29" s="137"/>
       <c r="R29" s="44" t="s">
@@ -7768,8 +7768,8 @@
         <v>27</v>
       </c>
       <c r="O40" s="148"/>
-      <c r="P40" s="131" t="s">
-        <v>197</v>
+      <c r="P40" s="51">
+        <v>45292</v>
       </c>
       <c r="Q40" s="149"/>
       <c r="R40" s="147"/>
@@ -7838,8 +7838,8 @@
       <c r="O41" s="244" t="s">
         <v>205</v>
       </c>
-      <c r="P41" s="242" t="s">
-        <v>197</v>
+      <c r="P41" s="51">
+        <v>45292</v>
       </c>
       <c r="Q41" s="239"/>
       <c r="R41" s="242" t="s">
@@ -8130,8 +8130,8 @@
         <v>23</v>
       </c>
       <c r="O45" s="47"/>
-      <c r="P45" s="44" t="s">
-        <v>197</v>
+      <c r="P45" s="51">
+        <v>45292</v>
       </c>
       <c r="Q45" s="41"/>
       <c r="R45" s="44" t="s">
@@ -9722,8 +9722,8 @@
       <c r="O67" s="63" t="s">
         <v>523</v>
       </c>
-      <c r="P67" s="44" t="s">
-        <v>197</v>
+      <c r="P67" s="51">
+        <v>45292</v>
       </c>
       <c r="Q67" s="41"/>
       <c r="R67" s="44"/>
@@ -13126,8 +13126,8 @@
       <c r="O114" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="P114" s="72" t="s">
-        <v>197</v>
+      <c r="P114" s="51">
+        <v>45292</v>
       </c>
       <c r="Q114" s="41"/>
       <c r="R114" s="44"/>
@@ -13566,8 +13566,8 @@
       <c r="O120" s="45" t="s">
         <v>509</v>
       </c>
-      <c r="P120" s="44" t="s">
-        <v>197</v>
+      <c r="P120" s="51">
+        <v>45292</v>
       </c>
       <c r="Q120" s="179" t="s">
         <v>27</v>
@@ -14478,8 +14478,8 @@
       <c r="O133" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="P133" s="44" t="s">
-        <v>197</v>
+      <c r="P133" s="51">
+        <v>45292</v>
       </c>
       <c r="Q133" s="41" t="s">
         <v>714</v>
@@ -16520,8 +16520,8 @@
       <c r="O161" s="73" t="s">
         <v>773</v>
       </c>
-      <c r="P161" s="51" t="s">
-        <v>197</v>
+      <c r="P161" s="51">
+        <v>45292</v>
       </c>
       <c r="Q161" s="137"/>
       <c r="R161" s="51" t="s">
@@ -16586,8 +16586,8 @@
         <v>23</v>
       </c>
       <c r="O162" s="47"/>
-      <c r="P162" s="44" t="s">
-        <v>197</v>
+      <c r="P162" s="51">
+        <v>45292</v>
       </c>
       <c r="Q162" s="41"/>
       <c r="R162" s="44" t="s">
@@ -17096,8 +17096,8 @@
       <c r="O169" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="P169" s="44" t="s">
-        <v>197</v>
+      <c r="P169" s="51">
+        <v>45292</v>
       </c>
       <c r="Q169" s="41"/>
       <c r="R169" s="44"/>
@@ -20148,8 +20148,8 @@
         <v>23</v>
       </c>
       <c r="O211" s="69"/>
-      <c r="P211" s="51" t="s">
-        <v>197</v>
+      <c r="P211" s="51">
+        <v>45292</v>
       </c>
       <c r="Q211" s="15"/>
       <c r="R211" s="51" t="s">
@@ -20212,8 +20212,8 @@
         <v>23</v>
       </c>
       <c r="O212" s="47"/>
-      <c r="P212" s="44" t="s">
-        <v>197</v>
+      <c r="P212" s="51">
+        <v>45292</v>
       </c>
       <c r="Q212" s="34"/>
       <c r="R212" s="44" t="s">
@@ -20428,8 +20428,8 @@
       <c r="O215" s="125" t="s">
         <v>959</v>
       </c>
-      <c r="P215" s="119" t="s">
-        <v>197</v>
+      <c r="P215" s="51">
+        <v>45292</v>
       </c>
       <c r="Q215" s="198"/>
       <c r="R215" s="119" t="s">
@@ -20480,8 +20480,8 @@
       <c r="M216" s="99"/>
       <c r="N216" s="99"/>
       <c r="O216" s="101"/>
-      <c r="P216" s="35" t="s">
-        <v>197</v>
+      <c r="P216" s="51">
+        <v>45292</v>
       </c>
       <c r="Q216" s="34"/>
       <c r="R216" s="104"/>
@@ -20696,8 +20696,8 @@
         <v>23</v>
       </c>
       <c r="O219" s="47"/>
-      <c r="P219" s="35" t="s">
-        <v>197</v>
+      <c r="P219" s="51">
+        <v>45292</v>
       </c>
       <c r="Q219" s="34"/>
       <c r="R219" s="102" t="s">
@@ -21872,8 +21872,8 @@
         <v>23</v>
       </c>
       <c r="O235" s="47"/>
-      <c r="P235" s="44" t="s">
-        <v>197</v>
+      <c r="P235" s="51">
+        <v>45292</v>
       </c>
       <c r="Q235" s="41"/>
       <c r="R235" s="44" t="s">
@@ -30252,7 +30252,7 @@
       </c>
       <c r="B338" s="1" t="e">
         <f>Dados_Onboarding!P11-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C338" s="1" t="e">
         <f>Dados_Onboarding!R11-Dados_Onboarding!H11</f>
@@ -30504,7 +30504,7 @@
       </c>
       <c r="B356" s="1" t="e">
         <f>Dados_Onboarding!P29-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C356" s="1" t="e">
         <f>Dados_Onboarding!R29-Dados_Onboarding!H29</f>
@@ -30658,7 +30658,7 @@
       </c>
       <c r="B367" s="1" t="e">
         <f>Dados_Onboarding!P40-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C367" s="1">
         <f>Dados_Onboarding!R40-Dados_Onboarding!H40</f>
@@ -30672,7 +30672,7 @@
       </c>
       <c r="B368" s="1" t="e">
         <f>Dados_Onboarding!P41-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C368" s="1" t="e">
         <f>Dados_Onboarding!R41-Dados_Onboarding!H41</f>
@@ -30728,7 +30728,7 @@
       </c>
       <c r="B372" s="1" t="e">
         <f>Dados_Onboarding!P45-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C372" s="1" t="e">
         <f>Dados_Onboarding!R45-Dados_Onboarding!H45</f>
@@ -31036,7 +31036,7 @@
       </c>
       <c r="B394" s="1" t="e">
         <f>Dados_Onboarding!P67-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C394" s="1">
         <f>Dados_Onboarding!R67-Dados_Onboarding!H67</f>
@@ -31694,7 +31694,7 @@
       </c>
       <c r="B441" s="1" t="e">
         <f>Dados_Onboarding!P114-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C441" s="1">
         <f>Dados_Onboarding!R114-Dados_Onboarding!H114</f>
@@ -31778,7 +31778,7 @@
       </c>
       <c r="B447" s="1" t="e">
         <f>Dados_Onboarding!P120-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C447" s="1" t="e">
         <f>Dados_Onboarding!R120-Dados_Onboarding!H120</f>
@@ -31960,7 +31960,7 @@
       </c>
       <c r="B460" s="1" t="e">
         <f>Dados_Onboarding!P133-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C460" s="1">
         <f>Dados_Onboarding!R133-Dados_Onboarding!H133</f>
@@ -32352,7 +32352,7 @@
       </c>
       <c r="B488" s="1" t="e">
         <f>Dados_Onboarding!P161-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C488" s="1" t="e">
         <f>Dados_Onboarding!R161-Dados_Onboarding!H161</f>
@@ -32366,7 +32366,7 @@
       </c>
       <c r="B489" s="1" t="e">
         <f>Dados_Onboarding!P162-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C489" s="1" t="e">
         <f>Dados_Onboarding!R162-Dados_Onboarding!H162</f>
@@ -32464,7 +32464,7 @@
       </c>
       <c r="B496" s="1" t="e">
         <f>Dados_Onboarding!P169-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C496" s="1">
         <f>Dados_Onboarding!R169-Dados_Onboarding!H169</f>
@@ -33052,7 +33052,7 @@
       </c>
       <c r="B538" s="1" t="e">
         <f>Dados_Onboarding!P211-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C538" s="1" t="e">
         <f>Dados_Onboarding!R211-Dados_Onboarding!H211</f>
@@ -33066,7 +33066,7 @@
       </c>
       <c r="B539" s="1" t="e">
         <f>Dados_Onboarding!P212-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C539" s="1" t="e">
         <f>Dados_Onboarding!R212-Dados_Onboarding!H212</f>
@@ -33108,7 +33108,7 @@
       </c>
       <c r="B542" s="1" t="e">
         <f>Dados_Onboarding!P215-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C542" s="1" t="e">
         <f>Dados_Onboarding!R215-Dados_Onboarding!H215</f>
@@ -33122,7 +33122,7 @@
       </c>
       <c r="B543" s="1" t="e">
         <f>Dados_Onboarding!P216-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C543" s="1">
         <f>Dados_Onboarding!R216-Dados_Onboarding!H216</f>
@@ -33164,7 +33164,7 @@
       </c>
       <c r="B546" s="1" t="e">
         <f>Dados_Onboarding!P219-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C546" s="1" t="e">
         <f>Dados_Onboarding!R219-Dados_Onboarding!H219</f>
@@ -33388,7 +33388,7 @@
       </c>
       <c r="B562" s="1" t="e">
         <f>Dados_Onboarding!P235-Dados_Onboarding!#REF!</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="C562" s="1" t="e">
         <f>Dados_Onboarding!R235-Dados_Onboarding!H235</f>
@@ -35108,6 +35108,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7271154-468d-4943-ad07-15f269a1f4f5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d241df49-fd27-41d8-ada8-b5e5272d8d25">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA29468F728387459F757BCD2E9F8EC0" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2a025e6ed7ca8ca0dee54093d0292095">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d241df49-fd27-41d8-ada8-b5e5272d8d25" xmlns:ns3="f7271154-468d-4943-ad07-15f269a1f4f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="07888a9383f211a4c31d7a2912379377" ns2:_="" ns3:_="">
     <xsd:import namespace="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
@@ -35356,27 +35376,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7271154-468d-4943-ad07-15f269a1f4f5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d241df49-fd27-41d8-ada8-b5e5272d8d25">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828E50A0-1F61-4B82-AF91-2402CEF44BFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7271154-468d-4943-ad07-15f269a1f4f5"/>
+    <ds:schemaRef ds:uri="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43F00D52-907D-4343-97A1-070EFC674BD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35393,23 +35412,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828E50A0-1F61-4B82-AF91-2402CEF44BFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7271154-468d-4943-ad07-15f269a1f4f5"/>
-    <ds:schemaRef ds:uri="d241df49-fd27-41d8-ada8-b5e5272d8d25"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2B58C3-6B57-4738-904D-545FBD745286}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>